<commit_message>
Pass data from the controller to the view
</commit_message>
<xml_diff>
--- a/me/4.Views.xlsx
+++ b/me/4.Views.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\build-php-mvc-framework\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9588D4C4-1CAD-4827-AA83-FB27C3988CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C49612-4CC7-4947-B6B6-6C46B51C677D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Display a view" sheetId="1" r:id="rId1"/>
+    <sheet name="PassDataFromControllerToView" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="95">
   <si>
     <t>Display a view: create a class to render views and use it in a controller</t>
   </si>
@@ -281,6 +282,113 @@
   </si>
   <si>
     <t>http://localhost/</t>
+  </si>
+  <si>
+    <t>Pass data from the controller to the view</t>
+  </si>
+  <si>
+    <t>        extract($args, EXTR_SKIP);</t>
+  </si>
+  <si>
+    <r>
+      <t>    public static function render($view</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, $args = []</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> $args là data được pass từ controller đến view</t>
+  </si>
+  <si>
+    <t>convert  $args từ array sang variable</t>
+  </si>
+  <si>
+    <t>            'name'    =&gt; 'Dave',</t>
+  </si>
+  <si>
+    <t>            'colours' =&gt; ['red', 'green', 'blue']</t>
+  </si>
+  <si>
+    <r>
+      <t>        View::render('Home/index.php'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, [</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>    ]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>    &lt;p&gt;Hello &lt;?php echo htmlspecialchars($name); ?&gt;!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;ul&gt;</t>
+  </si>
+  <si>
+    <t>        &lt;?php foreach ($colours as $colour) : ?&gt;</t>
+  </si>
+  <si>
+    <t>            &lt;li&gt;&lt;?php echo htmlspecialchars($colour); ?&gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>        &lt;?php endforeach; ?&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>htmlspecialchars dùng để escape các ký tự html</t>
+  </si>
+  <si>
+    <t>Check browser</t>
   </si>
 </sst>
 </file>
@@ -409,7 +517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -423,6 +531,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -433,9 +543,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,6 +868,214 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>532788</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>161625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD998E4C-DBAC-493A-AFD2-868233283C5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="619125" y="25384125"/>
+          <a:ext cx="4895238" cy="2400000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24DF7266-D15D-D550-6C4C-3CD73E22ECCB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2876550" y="8524875"/>
+          <a:ext cx="104775" cy="10601325"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95DF8336-7416-9BEA-8647-A43E18AD7FAD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1343025" y="19402425"/>
+          <a:ext cx="1743075" cy="3286125"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EBE133B-B208-59F0-097E-EC268C72B321}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1057275" y="19573875"/>
+          <a:ext cx="828675" cy="3743325"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1023,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="N127" sqref="N127"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,74 +1356,52 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="17"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="14" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="19"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14" t="s">
+      <c r="B7" s="5"/>
+      <c r="D7" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="19"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14" t="s">
+      <c r="B8" s="5"/>
+      <c r="E8" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="19"/>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="19" t="s">
+      <c r="B9" s="5"/>
+      <c r="F9" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="23" t="s">
+      <c r="B10" s="5"/>
+      <c r="E10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="19"/>
+      <c r="F10" s="6"/>
       <c r="G10" t="s">
         <v>23</v>
       </c>
@@ -1114,44 +1410,32 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14" t="s">
+      <c r="B11" s="5"/>
+      <c r="E11" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="19"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14" t="s">
+      <c r="B12" s="5"/>
+      <c r="D12" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="19"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14" t="s">
+      <c r="B13" s="5"/>
+      <c r="D13" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="19"/>
+      <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
+      <c r="B14" s="5"/>
       <c r="E14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="19"/>
+      <c r="F14" s="6"/>
       <c r="G14" t="s">
         <v>23</v>
       </c>
@@ -1163,11 +1447,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
+      <c r="B15" s="5"/>
       <c r="F15" s="8" t="s">
         <v>17</v>
       </c>
@@ -1179,44 +1459,32 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="14" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="19"/>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14" t="s">
+      <c r="B17" s="5"/>
+      <c r="D17" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="19"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14" t="s">
+      <c r="B18" s="5"/>
+      <c r="D18" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="19"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="14"/>
+      <c r="B19" s="5"/>
       <c r="D19" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="19"/>
+      <c r="F19" s="6"/>
       <c r="G19" t="s">
         <v>23</v>
       </c>
@@ -1225,54 +1493,41 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="14" t="s">
+      <c r="B20" s="5"/>
+      <c r="C20" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="19"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="14" t="s">
+      <c r="B21" s="5"/>
+      <c r="C21" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="19"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14" t="s">
+      <c r="B22" s="5"/>
+      <c r="D22" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="19"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14" t="s">
+      <c r="B23" s="5"/>
+      <c r="D23" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="19"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="21" t="s">
+      <c r="B24" s="10"/>
+      <c r="C24" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="22"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1292,280 +1547,150 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
       <c r="H29" s="6"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
       <c r="H30" s="6"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
       <c r="H31" s="6"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
       <c r="H32" s="6"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
       <c r="H33" s="6"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
       <c r="H34" s="6"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
       <c r="H35" s="6"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
       <c r="H36" s="6"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="5"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
       <c r="H37" s="6"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
       <c r="H38" s="6"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
       <c r="H39" s="6"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
       <c r="H40" s="6"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24"/>
-      <c r="G41" s="24"/>
       <c r="H41" s="6"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="24"/>
       <c r="H42" s="6"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
       <c r="H43" s="6"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
       <c r="H44" s="6"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
       <c r="H45" s="6"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
-      <c r="G46" s="24"/>
       <c r="H46" s="6"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="24"/>
       <c r="H47" s="6"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="5"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
       <c r="H48" s="6"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C49" s="24"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="24"/>
       <c r="H49" s="6"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="24"/>
       <c r="H50" s="6"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24"/>
-      <c r="G51" s="24"/>
       <c r="H51" s="6"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="24"/>
       <c r="H52" s="6"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C53" s="24"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24"/>
-      <c r="F53" s="24"/>
-      <c r="G53" s="24"/>
       <c r="H53" s="6"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C54" s="24"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="24"/>
-      <c r="F54" s="24"/>
-      <c r="G54" s="24"/>
       <c r="H54" s="6"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -1596,400 +1721,236 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B60" s="5"/>
-      <c r="C60" s="24"/>
-      <c r="D60" s="24"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24"/>
       <c r="G60" s="6"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B61" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C61" s="24"/>
-      <c r="D61" s="24"/>
-      <c r="E61" s="24"/>
-      <c r="F61" s="24"/>
       <c r="G61" s="6"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B62" s="5"/>
-      <c r="C62" s="24"/>
-      <c r="D62" s="24"/>
-      <c r="E62" s="24"/>
-      <c r="F62" s="24"/>
       <c r="G62" s="6"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B63" s="25" t="s">
+      <c r="B63" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C63" s="24"/>
-      <c r="D63" s="24"/>
-      <c r="E63" s="24"/>
-      <c r="F63" s="24"/>
       <c r="G63" s="6"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B64" s="5"/>
-      <c r="C64" s="24"/>
-      <c r="D64" s="24"/>
-      <c r="E64" s="24"/>
-      <c r="F64" s="24"/>
       <c r="G64" s="6"/>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C65" s="24"/>
-      <c r="D65" s="24"/>
-      <c r="E65" s="24"/>
-      <c r="F65" s="24"/>
       <c r="G65" s="6"/>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C66" s="24"/>
-      <c r="D66" s="24"/>
-      <c r="E66" s="24"/>
-      <c r="F66" s="24"/>
       <c r="G66" s="6"/>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C67" s="24"/>
-      <c r="D67" s="24"/>
-      <c r="E67" s="24"/>
-      <c r="F67" s="24"/>
       <c r="G67" s="6"/>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C68" s="24"/>
-      <c r="D68" s="24"/>
-      <c r="E68" s="24"/>
-      <c r="F68" s="24"/>
       <c r="G68" s="6"/>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C69" s="24"/>
-      <c r="D69" s="24"/>
-      <c r="E69" s="24"/>
-      <c r="F69" s="24"/>
       <c r="G69" s="6"/>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70" s="5"/>
-      <c r="C70" s="24"/>
-      <c r="D70" s="24"/>
-      <c r="E70" s="24"/>
-      <c r="F70" s="24"/>
       <c r="G70" s="6"/>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B71" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C71" s="24"/>
-      <c r="D71" s="24"/>
-      <c r="E71" s="24"/>
-      <c r="F71" s="24"/>
       <c r="G71" s="6"/>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B72" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C72" s="24"/>
-      <c r="D72" s="24"/>
-      <c r="E72" s="24"/>
-      <c r="F72" s="24"/>
       <c r="G72" s="6"/>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B73" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C73" s="24"/>
-      <c r="D73" s="24"/>
-      <c r="E73" s="24"/>
-      <c r="F73" s="24"/>
       <c r="G73" s="6"/>
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B74" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C74" s="24"/>
-      <c r="D74" s="24"/>
-      <c r="E74" s="24"/>
-      <c r="F74" s="24"/>
       <c r="G74" s="6"/>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B75" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C75" s="24"/>
-      <c r="D75" s="24"/>
-      <c r="E75" s="24"/>
-      <c r="F75" s="24"/>
       <c r="G75" s="6"/>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B76" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C76" s="24"/>
-      <c r="D76" s="24"/>
-      <c r="E76" s="24"/>
-      <c r="F76" s="24"/>
       <c r="G76" s="6"/>
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B77" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C77" s="24"/>
-      <c r="D77" s="24"/>
-      <c r="E77" s="24"/>
-      <c r="F77" s="24"/>
       <c r="G77" s="6"/>
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B78" s="25" t="s">
+      <c r="B78" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C78" s="24"/>
-      <c r="D78" s="24"/>
-      <c r="E78" s="24"/>
-      <c r="F78" s="24"/>
       <c r="G78" s="6"/>
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B79" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C79" s="24"/>
-      <c r="D79" s="24"/>
-      <c r="E79" s="24"/>
-      <c r="F79" s="24"/>
       <c r="G79" s="6"/>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B80" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C80" s="24"/>
-      <c r="D80" s="24"/>
-      <c r="E80" s="24"/>
-      <c r="F80" s="24"/>
       <c r="G80" s="6"/>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B81" s="5"/>
-      <c r="C81" s="24"/>
-      <c r="D81" s="24"/>
-      <c r="E81" s="24"/>
-      <c r="F81" s="24"/>
       <c r="G81" s="6"/>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C82" s="24"/>
-      <c r="D82" s="24"/>
-      <c r="E82" s="24"/>
-      <c r="F82" s="24"/>
       <c r="G82" s="6"/>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C83" s="24"/>
-      <c r="D83" s="24"/>
-      <c r="E83" s="24"/>
-      <c r="F83" s="24"/>
       <c r="G83" s="6"/>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C84" s="24"/>
-      <c r="D84" s="24"/>
-      <c r="E84" s="24"/>
-      <c r="F84" s="24"/>
       <c r="G84" s="6"/>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C85" s="24"/>
-      <c r="D85" s="24"/>
-      <c r="E85" s="24"/>
-      <c r="F85" s="24"/>
       <c r="G85" s="6"/>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B86" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C86" s="24"/>
-      <c r="D86" s="24"/>
-      <c r="E86" s="24"/>
-      <c r="F86" s="24"/>
       <c r="G86" s="6"/>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B87" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C87" s="24"/>
-      <c r="D87" s="24"/>
-      <c r="E87" s="24"/>
-      <c r="F87" s="24"/>
       <c r="G87" s="6"/>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B88" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C88" s="24"/>
-      <c r="D88" s="24"/>
-      <c r="E88" s="24"/>
-      <c r="F88" s="24"/>
       <c r="G88" s="6"/>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B89" s="25" t="s">
+      <c r="B89" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C89" s="24"/>
-      <c r="D89" s="24"/>
-      <c r="E89" s="24"/>
-      <c r="F89" s="24"/>
       <c r="G89" s="6"/>
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C90" s="24"/>
-      <c r="D90" s="24"/>
-      <c r="E90" s="24"/>
-      <c r="F90" s="24"/>
       <c r="G90" s="6"/>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B91" s="5"/>
-      <c r="C91" s="24"/>
-      <c r="D91" s="24"/>
-      <c r="E91" s="24"/>
-      <c r="F91" s="24"/>
       <c r="G91" s="6"/>
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B92" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C92" s="24"/>
-      <c r="D92" s="24"/>
-      <c r="E92" s="24"/>
-      <c r="F92" s="24"/>
       <c r="G92" s="6"/>
     </row>
     <row r="93" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B93" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C93" s="24"/>
-      <c r="D93" s="24"/>
-      <c r="E93" s="24"/>
-      <c r="F93" s="24"/>
       <c r="G93" s="6"/>
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B94" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C94" s="24"/>
-      <c r="D94" s="24"/>
-      <c r="E94" s="24"/>
-      <c r="F94" s="24"/>
       <c r="G94" s="6"/>
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B95" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C95" s="24"/>
-      <c r="D95" s="24"/>
-      <c r="E95" s="24"/>
-      <c r="F95" s="24"/>
       <c r="G95" s="6"/>
     </row>
     <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B96" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C96" s="24"/>
-      <c r="D96" s="24"/>
-      <c r="E96" s="24"/>
-      <c r="F96" s="24"/>
       <c r="G96" s="6"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B97" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C97" s="24"/>
-      <c r="D97" s="24"/>
-      <c r="E97" s="24"/>
-      <c r="F97" s="24"/>
       <c r="G97" s="6"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B98" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C98" s="24"/>
-      <c r="D98" s="24"/>
-      <c r="E98" s="24"/>
-      <c r="F98" s="24"/>
       <c r="G98" s="6"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B99" s="25" t="s">
+      <c r="B99" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C99" s="24"/>
-      <c r="D99" s="24"/>
-      <c r="E99" s="24"/>
-      <c r="F99" s="24"/>
       <c r="G99" s="6"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B100" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C100" s="24"/>
-      <c r="D100" s="24"/>
-      <c r="E100" s="24"/>
-      <c r="F100" s="24"/>
       <c r="G100" s="6"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -2020,102 +1981,66 @@
       <c r="B106" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C106" s="24"/>
-      <c r="D106" s="24"/>
-      <c r="E106" s="24"/>
       <c r="F106" s="6"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B107" s="5"/>
-      <c r="C107" s="24"/>
-      <c r="D107" s="24"/>
-      <c r="E107" s="24"/>
       <c r="F107" s="6"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B108" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C108" s="24"/>
-      <c r="D108" s="24"/>
-      <c r="E108" s="24"/>
       <c r="F108" s="6"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B109" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C109" s="24"/>
-      <c r="D109" s="24"/>
-      <c r="E109" s="24"/>
       <c r="F109" s="6"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B110" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C110" s="24"/>
-      <c r="D110" s="24"/>
-      <c r="E110" s="24"/>
       <c r="F110" s="6"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B111" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C111" s="24"/>
-      <c r="D111" s="24"/>
-      <c r="E111" s="24"/>
       <c r="F111" s="6"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B112" s="5"/>
-      <c r="C112" s="24"/>
-      <c r="D112" s="24"/>
-      <c r="E112" s="24"/>
       <c r="F112" s="6"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B113" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C113" s="24"/>
-      <c r="D113" s="24"/>
-      <c r="E113" s="24"/>
       <c r="F113" s="6"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B114" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C114" s="24"/>
-      <c r="D114" s="24"/>
-      <c r="E114" s="24"/>
       <c r="F114" s="6"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B115" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C115" s="24"/>
-      <c r="D115" s="24"/>
-      <c r="E115" s="24"/>
       <c r="F115" s="6"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B116" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C116" s="24"/>
-      <c r="D116" s="24"/>
-      <c r="E116" s="24"/>
       <c r="F116" s="6"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B117" s="5"/>
-      <c r="C117" s="24"/>
-      <c r="D117" s="24"/>
-      <c r="E117" s="24"/>
       <c r="F117" s="6"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -2136,6 +2061,1431 @@
       <c r="B122" s="9" t="s">
         <v>77</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B19F77-1B28-4159-8475-E4EC1188D53C}">
+  <dimension ref="A2:J147"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="N104" sqref="N104"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="19"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="21"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="21"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="21"/>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="21"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="16"/>
+      <c r="F12" s="21"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="16"/>
+      <c r="F13" s="21"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="21"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="21"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="16"/>
+      <c r="F17" s="21"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="16"/>
+      <c r="F18" s="21"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="21"/>
+      <c r="G19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="16"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="21"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="21"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="16"/>
+      <c r="F22" s="21"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="16"/>
+      <c r="F23" s="21"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="24"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="5"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="6"/>
+      <c r="I45" t="s">
+        <v>23</v>
+      </c>
+      <c r="J45" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
+      <c r="H47" s="6"/>
+      <c r="I47" t="s">
+        <v>23</v>
+      </c>
+      <c r="J47" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="5"/>
+      <c r="C48" s="25"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="6"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="25"/>
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="5"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="25"/>
+      <c r="G50" s="25"/>
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" s="25"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="6"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C52" s="25"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="25"/>
+      <c r="G52" s="25"/>
+      <c r="H52" s="6"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="25"/>
+      <c r="H53" s="6"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="25"/>
+      <c r="G54" s="25"/>
+      <c r="H54" s="6"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="25"/>
+      <c r="H55" s="6"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C56" s="25"/>
+      <c r="D56" s="25"/>
+      <c r="E56" s="25"/>
+      <c r="F56" s="25"/>
+      <c r="G56" s="25"/>
+      <c r="H56" s="6"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="12"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="4"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="5"/>
+      <c r="C62" s="25"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="25"/>
+      <c r="F62" s="25"/>
+      <c r="G62" s="6"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C63" s="25"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="25"/>
+      <c r="F63" s="25"/>
+      <c r="G63" s="6"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="5"/>
+      <c r="C64" s="25"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="25"/>
+      <c r="F64" s="25"/>
+      <c r="G64" s="6"/>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C65" s="25"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="25"/>
+      <c r="F65" s="25"/>
+      <c r="G65" s="6"/>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" s="5"/>
+      <c r="C66" s="25"/>
+      <c r="D66" s="25"/>
+      <c r="E66" s="25"/>
+      <c r="F66" s="25"/>
+      <c r="G66" s="6"/>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C67" s="25"/>
+      <c r="D67" s="25"/>
+      <c r="E67" s="25"/>
+      <c r="F67" s="25"/>
+      <c r="G67" s="6"/>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C68" s="25"/>
+      <c r="D68" s="25"/>
+      <c r="E68" s="25"/>
+      <c r="F68" s="25"/>
+      <c r="G68" s="6"/>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B69" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C69" s="25"/>
+      <c r="D69" s="25"/>
+      <c r="E69" s="25"/>
+      <c r="F69" s="25"/>
+      <c r="G69" s="6"/>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C70" s="25"/>
+      <c r="D70" s="25"/>
+      <c r="E70" s="25"/>
+      <c r="F70" s="25"/>
+      <c r="G70" s="6"/>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C71" s="25"/>
+      <c r="D71" s="25"/>
+      <c r="E71" s="25"/>
+      <c r="F71" s="25"/>
+      <c r="G71" s="6"/>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B72" s="5"/>
+      <c r="C72" s="25"/>
+      <c r="D72" s="25"/>
+      <c r="E72" s="25"/>
+      <c r="F72" s="25"/>
+      <c r="G72" s="6"/>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B73" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C73" s="25"/>
+      <c r="D73" s="25"/>
+      <c r="E73" s="25"/>
+      <c r="F73" s="25"/>
+      <c r="G73" s="6"/>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B74" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C74" s="25"/>
+      <c r="D74" s="25"/>
+      <c r="E74" s="25"/>
+      <c r="F74" s="25"/>
+      <c r="G74" s="6"/>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B75" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C75" s="25"/>
+      <c r="D75" s="25"/>
+      <c r="E75" s="25"/>
+      <c r="F75" s="25"/>
+      <c r="G75" s="6"/>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B76" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C76" s="25"/>
+      <c r="D76" s="25"/>
+      <c r="E76" s="25"/>
+      <c r="F76" s="25"/>
+      <c r="G76" s="6"/>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B77" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C77" s="25"/>
+      <c r="D77" s="25"/>
+      <c r="E77" s="25"/>
+      <c r="F77" s="25"/>
+      <c r="G77" s="6"/>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B78" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C78" s="25"/>
+      <c r="D78" s="25"/>
+      <c r="E78" s="25"/>
+      <c r="F78" s="25"/>
+      <c r="G78" s="6"/>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B79" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C79" s="25"/>
+      <c r="D79" s="25"/>
+      <c r="E79" s="25"/>
+      <c r="F79" s="25"/>
+      <c r="G79" s="6"/>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B80" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C80" s="25"/>
+      <c r="D80" s="25"/>
+      <c r="E80" s="25"/>
+      <c r="F80" s="25"/>
+      <c r="G80" s="6"/>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B81" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C81" s="25"/>
+      <c r="D81" s="25"/>
+      <c r="E81" s="25"/>
+      <c r="F81" s="25"/>
+      <c r="G81" s="6"/>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B82" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C82" s="25"/>
+      <c r="D82" s="25"/>
+      <c r="E82" s="25"/>
+      <c r="F82" s="25"/>
+      <c r="G82" s="6"/>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B83" s="5"/>
+      <c r="C83" s="25"/>
+      <c r="D83" s="25"/>
+      <c r="E83" s="25"/>
+      <c r="F83" s="25"/>
+      <c r="G83" s="6"/>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B84" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C84" s="25"/>
+      <c r="D84" s="25"/>
+      <c r="E84" s="25"/>
+      <c r="F84" s="25"/>
+      <c r="G84" s="6"/>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B85" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C85" s="25"/>
+      <c r="D85" s="25"/>
+      <c r="E85" s="25"/>
+      <c r="F85" s="25"/>
+      <c r="G85" s="6"/>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B86" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C86" s="25"/>
+      <c r="D86" s="25"/>
+      <c r="E86" s="25"/>
+      <c r="F86" s="25"/>
+      <c r="G86" s="6"/>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B87" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C87" s="25"/>
+      <c r="D87" s="25"/>
+      <c r="E87" s="25"/>
+      <c r="F87" s="25"/>
+      <c r="G87" s="6"/>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B88" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C88" s="25"/>
+      <c r="D88" s="25"/>
+      <c r="E88" s="25"/>
+      <c r="F88" s="25"/>
+      <c r="G88" s="6"/>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B89" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C89" s="25"/>
+      <c r="D89" s="25"/>
+      <c r="E89" s="25"/>
+      <c r="F89" s="25"/>
+      <c r="G89" s="6"/>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B90" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C90" s="25"/>
+      <c r="D90" s="25"/>
+      <c r="E90" s="25"/>
+      <c r="F90" s="25"/>
+      <c r="G90" s="6"/>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B91" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C91" s="25"/>
+      <c r="D91" s="25"/>
+      <c r="E91" s="25"/>
+      <c r="F91" s="25"/>
+      <c r="G91" s="6"/>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B92" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C92" s="25"/>
+      <c r="D92" s="25"/>
+      <c r="E92" s="25"/>
+      <c r="F92" s="25"/>
+      <c r="G92" s="6"/>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="5"/>
+      <c r="C93" s="25"/>
+      <c r="D93" s="25"/>
+      <c r="E93" s="25"/>
+      <c r="F93" s="25"/>
+      <c r="G93" s="6"/>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B94" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C94" s="25"/>
+      <c r="D94" s="25"/>
+      <c r="E94" s="25"/>
+      <c r="F94" s="25"/>
+      <c r="G94" s="6"/>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B95" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C95" s="25"/>
+      <c r="D95" s="25"/>
+      <c r="E95" s="25"/>
+      <c r="F95" s="25"/>
+      <c r="G95" s="6"/>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B96" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C96" s="25"/>
+      <c r="D96" s="25"/>
+      <c r="E96" s="25"/>
+      <c r="F96" s="25"/>
+      <c r="G96" s="6"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B97" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C97" s="25"/>
+      <c r="D97" s="25"/>
+      <c r="E97" s="25"/>
+      <c r="F97" s="25"/>
+      <c r="G97" s="6"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B98" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C98" s="25"/>
+      <c r="D98" s="25"/>
+      <c r="E98" s="25"/>
+      <c r="F98" s="25"/>
+      <c r="G98" s="6"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B99" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C99" s="25"/>
+      <c r="D99" s="25"/>
+      <c r="E99" s="25"/>
+      <c r="F99" s="25"/>
+      <c r="G99" s="6"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B100" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C100" s="25"/>
+      <c r="D100" s="25"/>
+      <c r="E100" s="25"/>
+      <c r="F100" s="25"/>
+      <c r="G100" s="6"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B101" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C101" s="25"/>
+      <c r="D101" s="25"/>
+      <c r="E101" s="25"/>
+      <c r="F101" s="25"/>
+      <c r="G101" s="6"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B102" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C102" s="25"/>
+      <c r="D102" s="25"/>
+      <c r="E102" s="25"/>
+      <c r="F102" s="25"/>
+      <c r="G102" s="6"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B103" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C103" s="25"/>
+      <c r="D103" s="25"/>
+      <c r="E103" s="25"/>
+      <c r="F103" s="25"/>
+      <c r="G103" s="6"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B104" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C104" s="25"/>
+      <c r="D104" s="25"/>
+      <c r="E104" s="25"/>
+      <c r="F104" s="25"/>
+      <c r="G104" s="6"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B105" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C105" s="25"/>
+      <c r="D105" s="25"/>
+      <c r="E105" s="25"/>
+      <c r="F105" s="25"/>
+      <c r="G105" s="6"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B106" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C106" s="11"/>
+      <c r="D106" s="11"/>
+      <c r="E106" s="11"/>
+      <c r="F106" s="11"/>
+      <c r="G106" s="12"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B110" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C110" s="3"/>
+      <c r="D110" s="3"/>
+      <c r="E110" s="3"/>
+      <c r="F110" s="3"/>
+      <c r="G110" s="4"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B111" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C111" s="25"/>
+      <c r="D111" s="25"/>
+      <c r="E111" s="25"/>
+      <c r="F111" s="25"/>
+      <c r="G111" s="6"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B112" s="5"/>
+      <c r="C112" s="25"/>
+      <c r="D112" s="25"/>
+      <c r="E112" s="25"/>
+      <c r="F112" s="25"/>
+      <c r="G112" s="6"/>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B113" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C113" s="25"/>
+      <c r="D113" s="25"/>
+      <c r="E113" s="25"/>
+      <c r="F113" s="25"/>
+      <c r="G113" s="6"/>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B114" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C114" s="25"/>
+      <c r="D114" s="25"/>
+      <c r="E114" s="25"/>
+      <c r="F114" s="25"/>
+      <c r="G114" s="6"/>
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B115" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C115" s="25"/>
+      <c r="D115" s="25"/>
+      <c r="E115" s="25"/>
+      <c r="F115" s="25"/>
+      <c r="G115" s="6"/>
+    </row>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B116" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C116" s="25"/>
+      <c r="D116" s="25"/>
+      <c r="E116" s="25"/>
+      <c r="F116" s="25"/>
+      <c r="G116" s="6"/>
+    </row>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B117" s="5"/>
+      <c r="C117" s="25"/>
+      <c r="D117" s="25"/>
+      <c r="E117" s="25"/>
+      <c r="F117" s="25"/>
+      <c r="G117" s="6"/>
+    </row>
+    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B118" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C118" s="25"/>
+      <c r="D118" s="25"/>
+      <c r="E118" s="25"/>
+      <c r="F118" s="25"/>
+      <c r="G118" s="6"/>
+    </row>
+    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B119" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C119" s="25"/>
+      <c r="D119" s="25"/>
+      <c r="E119" s="25"/>
+      <c r="F119" s="25"/>
+      <c r="G119" s="6"/>
+    </row>
+    <row r="120" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B120" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C120" s="25"/>
+      <c r="D120" s="25"/>
+      <c r="E120" s="25"/>
+      <c r="F120" s="25"/>
+      <c r="G120" s="6"/>
+      <c r="H120" t="s">
+        <v>23</v>
+      </c>
+      <c r="I120" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B121" s="14"/>
+      <c r="C121" s="25"/>
+      <c r="D121" s="25"/>
+      <c r="E121" s="25"/>
+      <c r="F121" s="25"/>
+      <c r="G121" s="6"/>
+    </row>
+    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B122" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C122" s="25"/>
+      <c r="D122" s="25"/>
+      <c r="E122" s="25"/>
+      <c r="F122" s="25"/>
+      <c r="G122" s="6"/>
+    </row>
+    <row r="123" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B123" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C123" s="25"/>
+      <c r="D123" s="25"/>
+      <c r="E123" s="25"/>
+      <c r="F123" s="25"/>
+      <c r="G123" s="6"/>
+    </row>
+    <row r="124" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B124" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C124" s="25"/>
+      <c r="D124" s="25"/>
+      <c r="E124" s="25"/>
+      <c r="F124" s="25"/>
+      <c r="G124" s="6"/>
+    </row>
+    <row r="125" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B125" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C125" s="25"/>
+      <c r="D125" s="25"/>
+      <c r="E125" s="25"/>
+      <c r="F125" s="25"/>
+      <c r="G125" s="6"/>
+    </row>
+    <row r="126" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B126" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C126" s="25"/>
+      <c r="D126" s="25"/>
+      <c r="E126" s="25"/>
+      <c r="F126" s="25"/>
+      <c r="G126" s="6"/>
+    </row>
+    <row r="127" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B127" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C127" s="25"/>
+      <c r="D127" s="25"/>
+      <c r="E127" s="25"/>
+      <c r="F127" s="25"/>
+      <c r="G127" s="6"/>
+    </row>
+    <row r="128" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B128" s="5"/>
+      <c r="C128" s="25"/>
+      <c r="D128" s="25"/>
+      <c r="E128" s="25"/>
+      <c r="F128" s="25"/>
+      <c r="G128" s="6"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B129" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C129" s="11"/>
+      <c r="D129" s="11"/>
+      <c r="E129" s="11"/>
+      <c r="F129" s="11"/>
+      <c r="G129" s="12"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="B132" s="3"/>
+      <c r="C132" s="3"/>
+      <c r="D132" s="3"/>
+      <c r="E132" s="3"/>
+      <c r="F132" s="3"/>
+      <c r="G132" s="3"/>
+      <c r="H132" s="3"/>
+      <c r="I132" s="4"/>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A133" s="5"/>
+      <c r="B133" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C133" s="25"/>
+      <c r="D133" s="25"/>
+      <c r="E133" s="25"/>
+      <c r="F133" s="25"/>
+      <c r="G133" s="25"/>
+      <c r="H133" s="25"/>
+      <c r="I133" s="6"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134" s="5"/>
+      <c r="B134" s="25"/>
+      <c r="C134" s="25"/>
+      <c r="D134" s="25"/>
+      <c r="E134" s="25"/>
+      <c r="F134" s="25"/>
+      <c r="G134" s="25"/>
+      <c r="H134" s="25"/>
+      <c r="I134" s="6"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" s="5"/>
+      <c r="B135" s="25"/>
+      <c r="C135" s="25"/>
+      <c r="D135" s="25"/>
+      <c r="E135" s="25"/>
+      <c r="F135" s="25"/>
+      <c r="G135" s="25"/>
+      <c r="H135" s="25"/>
+      <c r="I135" s="6"/>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" s="5"/>
+      <c r="B136" s="25"/>
+      <c r="C136" s="25"/>
+      <c r="D136" s="25"/>
+      <c r="E136" s="25"/>
+      <c r="F136" s="25"/>
+      <c r="G136" s="25"/>
+      <c r="H136" s="25"/>
+      <c r="I136" s="6"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137" s="5"/>
+      <c r="B137" s="25"/>
+      <c r="C137" s="25"/>
+      <c r="D137" s="25"/>
+      <c r="E137" s="25"/>
+      <c r="F137" s="25"/>
+      <c r="G137" s="25"/>
+      <c r="H137" s="25"/>
+      <c r="I137" s="6"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138" s="5"/>
+      <c r="B138" s="25"/>
+      <c r="C138" s="25"/>
+      <c r="D138" s="25"/>
+      <c r="E138" s="25"/>
+      <c r="F138" s="25"/>
+      <c r="G138" s="25"/>
+      <c r="H138" s="25"/>
+      <c r="I138" s="6"/>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A139" s="5"/>
+      <c r="B139" s="25"/>
+      <c r="C139" s="25"/>
+      <c r="D139" s="25"/>
+      <c r="E139" s="25"/>
+      <c r="F139" s="25"/>
+      <c r="G139" s="25"/>
+      <c r="H139" s="25"/>
+      <c r="I139" s="6"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A140" s="5"/>
+      <c r="B140" s="25"/>
+      <c r="C140" s="25"/>
+      <c r="D140" s="25"/>
+      <c r="E140" s="25"/>
+      <c r="F140" s="25"/>
+      <c r="G140" s="25"/>
+      <c r="H140" s="25"/>
+      <c r="I140" s="6"/>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A141" s="5"/>
+      <c r="B141" s="25"/>
+      <c r="C141" s="25"/>
+      <c r="D141" s="25"/>
+      <c r="E141" s="25"/>
+      <c r="F141" s="25"/>
+      <c r="G141" s="25"/>
+      <c r="H141" s="25"/>
+      <c r="I141" s="6"/>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A142" s="5"/>
+      <c r="B142" s="25"/>
+      <c r="C142" s="25"/>
+      <c r="D142" s="25"/>
+      <c r="E142" s="25"/>
+      <c r="F142" s="25"/>
+      <c r="G142" s="25"/>
+      <c r="H142" s="25"/>
+      <c r="I142" s="6"/>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143" s="5"/>
+      <c r="B143" s="25"/>
+      <c r="C143" s="25"/>
+      <c r="D143" s="25"/>
+      <c r="E143" s="25"/>
+      <c r="F143" s="25"/>
+      <c r="G143" s="25"/>
+      <c r="H143" s="25"/>
+      <c r="I143" s="6"/>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A144" s="5"/>
+      <c r="B144" s="25"/>
+      <c r="C144" s="25"/>
+      <c r="D144" s="25"/>
+      <c r="E144" s="25"/>
+      <c r="F144" s="25"/>
+      <c r="G144" s="25"/>
+      <c r="H144" s="25"/>
+      <c r="I144" s="6"/>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A145" s="5"/>
+      <c r="B145" s="25"/>
+      <c r="C145" s="25"/>
+      <c r="D145" s="25"/>
+      <c r="E145" s="25"/>
+      <c r="F145" s="25"/>
+      <c r="G145" s="25"/>
+      <c r="H145" s="25"/>
+      <c r="I145" s="6"/>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A146" s="5"/>
+      <c r="B146" s="25"/>
+      <c r="C146" s="25"/>
+      <c r="D146" s="25"/>
+      <c r="E146" s="25"/>
+      <c r="F146" s="25"/>
+      <c r="G146" s="25"/>
+      <c r="H146" s="25"/>
+      <c r="I146" s="6"/>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A147" s="10"/>
+      <c r="B147" s="11"/>
+      <c r="C147" s="11"/>
+      <c r="D147" s="11"/>
+      <c r="E147" s="11"/>
+      <c r="F147" s="11"/>
+      <c r="G147" s="11"/>
+      <c r="H147" s="11"/>
+      <c r="I147" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Make views easier to create and maintain: add a template engine
</commit_message>
<xml_diff>
--- a/me/4.Views.xlsx
+++ b/me/4.Views.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\build-php-mvc-framework\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C49612-4CC7-4947-B6B6-6C46B51C677D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F57235C-AEC2-45AA-AF5D-E59AC0358C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Display a view" sheetId="1" r:id="rId1"/>
     <sheet name="PassDataFromControllerToView" sheetId="2" r:id="rId2"/>
+    <sheet name="add a template engine" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="124">
   <si>
     <t>Display a view: create a class to render views and use it in a controller</t>
   </si>
@@ -389,6 +390,135 @@
   </si>
   <si>
     <t>Check browser</t>
+  </si>
+  <si>
+    <t>Make views easier to create and maintain: add a template engine</t>
+  </si>
+  <si>
+    <t>composer require "twig/twig:^3.0"</t>
+  </si>
+  <si>
+    <t>twig</t>
+  </si>
+  <si>
+    <t>https://twig.symfony.com/doc/3.x/intro.html</t>
+  </si>
+  <si>
+    <t>index.html</t>
+  </si>
+  <si>
+    <t>    public static function render($view, $args = [])</t>
+  </si>
+  <si>
+    <t>     * Render a view template using Twig</t>
+  </si>
+  <si>
+    <t>     * @param string $template  The template file</t>
+  </si>
+  <si>
+    <t>     * @param array $args  Associative array of data to display in the view (optional)</t>
+  </si>
+  <si>
+    <t>    public static function renderTemplate($template, $args = [])</t>
+  </si>
+  <si>
+    <t>        $twig = new \Twig\Environment($loader);</t>
+  </si>
+  <si>
+    <t>        ]);</t>
+  </si>
+  <si>
+    <t>build-php-mvc-framework\App\Views\Home\index.html</t>
+  </si>
+  <si>
+    <t>    &lt;head&gt;</t>
+  </si>
+  <si>
+    <t>        &lt;meta charset="UTF-8" /&gt;</t>
+  </si>
+  <si>
+    <t>        &lt;title&gt;Home&lt;/title&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;/head&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;body&gt;</t>
+  </si>
+  <si>
+    <t>        &lt;h1&gt;Welcome&lt;/h1&gt;</t>
+  </si>
+  <si>
+    <t>        &lt;p&gt;Hello from a Twig template, {{ name }}!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>        &lt;ul&gt;</t>
+  </si>
+  <si>
+    <t>        {% for colour in colours %}</t>
+  </si>
+  <si>
+    <t>        &lt;li&gt;{{ colour }}&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>        {% endfor %}</t>
+  </si>
+  <si>
+    <t>        &lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;/body&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t>        View::render</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Template</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>('Home/index.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>', [</t>
+    </r>
+  </si>
+  <si>
+    <t>        $loader = new \Twig\Loader\FilesystemLoader("../App/Views");</t>
+  </si>
+  <si>
+    <t>        echo $twig-&gt;render($template, $args);</t>
   </si>
 </sst>
 </file>
@@ -517,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -533,19 +663,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1076,6 +1196,381 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>151459</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>37651</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F784D65-E8EC-2786-6D40-55A736FA49DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695325" y="6924675"/>
+          <a:ext cx="7523809" cy="3590476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>27269</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>18830</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5456B8E-BD9F-39E6-D4C1-5CF6E2450B8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695325" y="923925"/>
+          <a:ext cx="10447619" cy="1761905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>322592</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>56769</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F580B3DA-885A-3C9F-B152-CB75AF65DB35}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="3105150"/>
+          <a:ext cx="10066667" cy="3047619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EB763CA-C172-A9BE-C15C-39120D7D2371}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="857250" y="2495550"/>
+          <a:ext cx="476250" cy="8791575"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>342581</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>113744</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85A06492-FE18-B5B2-D1DB-B20AC914AC31}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="838200" y="15287625"/>
+          <a:ext cx="2552381" cy="4447619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3129AF28-2BC4-3E1A-409B-2821AF8F8D12}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1095375" y="4572000"/>
+          <a:ext cx="523875" cy="23526750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>226</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>161439</xdr:colOff>
+      <xdr:row>238</xdr:row>
+      <xdr:rowOff>133057</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71437120-D7A0-7A1B-D973-B59E62A916A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="43129200"/>
+          <a:ext cx="3885714" cy="2342857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>193</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>236718</xdr:colOff>
+      <xdr:row>201</xdr:row>
+      <xdr:rowOff>133154</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9D86DDB-757B-9B43-0E81-803DDD5A8F74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4972050" y="36852225"/>
+          <a:ext cx="11257143" cy="1571429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2072,8 +2567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B19F77-1B28-4159-8475-E4EC1188D53C}">
   <dimension ref="A2:J147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="N104" sqref="N104"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2087,74 +2582,52 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="19"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="16" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="21"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16" t="s">
+      <c r="B7" s="5"/>
+      <c r="D7" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="21"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16" t="s">
+      <c r="B8" s="5"/>
+      <c r="E8" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="21" t="s">
+      <c r="B9" s="5"/>
+      <c r="F9" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
+      <c r="B10" s="5"/>
       <c r="E10" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="6"/>
       <c r="G10" t="s">
         <v>23</v>
       </c>
@@ -2163,51 +2636,35 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16" t="s">
+      <c r="B11" s="5"/>
+      <c r="E11" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="21"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16" t="s">
+      <c r="B12" s="5"/>
+      <c r="D12" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="21"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16" t="s">
+      <c r="B13" s="5"/>
+      <c r="D13" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="21"/>
+      <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16" t="s">
+      <c r="B14" s="5"/>
+      <c r="E14" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="21"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
+      <c r="B15" s="5"/>
       <c r="F15" s="8" t="s">
         <v>17</v>
       </c>
@@ -2219,44 +2676,32 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="16" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="21"/>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16" t="s">
+      <c r="B17" s="5"/>
+      <c r="D17" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="21"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16" t="s">
+      <c r="B18" s="5"/>
+      <c r="D18" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="21"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="16"/>
+      <c r="B19" s="5"/>
       <c r="D19" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="21"/>
+      <c r="F19" s="6"/>
       <c r="G19" t="s">
         <v>23</v>
       </c>
@@ -2265,54 +2710,41 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="16" t="s">
+      <c r="B20" s="5"/>
+      <c r="C20" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="21"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="16" t="s">
+      <c r="B21" s="5"/>
+      <c r="C21" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="21"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16" t="s">
+      <c r="B22" s="5"/>
+      <c r="D22" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="16"/>
-      <c r="F22" s="21"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16" t="s">
+      <c r="B23" s="5"/>
+      <c r="D23" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="16"/>
-      <c r="F23" s="21"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="23" t="s">
+      <c r="B24" s="10"/>
+      <c r="C24" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="24"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -2332,183 +2764,98 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
       <c r="H29" s="6"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
       <c r="H30" s="6"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
       <c r="H31" s="6"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
       <c r="H32" s="6"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
       <c r="H33" s="6"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
       <c r="H34" s="6"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
       <c r="H35" s="6"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
       <c r="H36" s="6"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="5"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
       <c r="H37" s="6"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
       <c r="H38" s="6"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
       <c r="H39" s="6"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
       <c r="H40" s="6"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
       <c r="H41" s="6"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25"/>
       <c r="H42" s="6"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
       <c r="H43" s="6"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
       <c r="H44" s="6"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
       <c r="H45" s="6"/>
       <c r="I45" t="s">
         <v>23</v>
@@ -2521,22 +2868,12 @@
       <c r="B46" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25"/>
       <c r="H46" s="6"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
       <c r="H47" s="6"/>
       <c r="I47" t="s">
         <v>23</v>
@@ -2547,97 +2884,52 @@
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="5"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
       <c r="H48" s="6"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
       <c r="H49" s="6"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B50" s="5"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="25"/>
       <c r="H50" s="6"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C51" s="25"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
-      <c r="F51" s="25"/>
-      <c r="G51" s="25"/>
       <c r="H51" s="6"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="25"/>
-      <c r="G52" s="25"/>
       <c r="H52" s="6"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
       <c r="H53" s="6"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="25"/>
       <c r="H54" s="6"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="25"/>
       <c r="H55" s="6"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C56" s="25"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="25"/>
-      <c r="F56" s="25"/>
-      <c r="G56" s="25"/>
       <c r="H56" s="6"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -2668,430 +2960,254 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B62" s="5"/>
-      <c r="C62" s="25"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="25"/>
       <c r="G62" s="6"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B63" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="25"/>
       <c r="G63" s="6"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B64" s="5"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25"/>
       <c r="G64" s="6"/>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
       <c r="G65" s="6"/>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66" s="5"/>
-      <c r="C66" s="25"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="25"/>
-      <c r="F66" s="25"/>
       <c r="G66" s="6"/>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C67" s="25"/>
-      <c r="D67" s="25"/>
-      <c r="E67" s="25"/>
-      <c r="F67" s="25"/>
       <c r="G67" s="6"/>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="25"/>
       <c r="G68" s="6"/>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C69" s="25"/>
-      <c r="D69" s="25"/>
-      <c r="E69" s="25"/>
-      <c r="F69" s="25"/>
       <c r="G69" s="6"/>
     </row>
     <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C70" s="25"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="25"/>
-      <c r="F70" s="25"/>
       <c r="G70" s="6"/>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B71" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C71" s="25"/>
-      <c r="D71" s="25"/>
-      <c r="E71" s="25"/>
-      <c r="F71" s="25"/>
       <c r="G71" s="6"/>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B72" s="5"/>
-      <c r="C72" s="25"/>
-      <c r="D72" s="25"/>
-      <c r="E72" s="25"/>
-      <c r="F72" s="25"/>
       <c r="G72" s="6"/>
     </row>
     <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B73" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C73" s="25"/>
-      <c r="D73" s="25"/>
-      <c r="E73" s="25"/>
-      <c r="F73" s="25"/>
       <c r="G73" s="6"/>
     </row>
     <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B74" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C74" s="25"/>
-      <c r="D74" s="25"/>
-      <c r="E74" s="25"/>
-      <c r="F74" s="25"/>
       <c r="G74" s="6"/>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B75" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C75" s="25"/>
-      <c r="D75" s="25"/>
-      <c r="E75" s="25"/>
-      <c r="F75" s="25"/>
       <c r="G75" s="6"/>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B76" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C76" s="25"/>
-      <c r="D76" s="25"/>
-      <c r="E76" s="25"/>
-      <c r="F76" s="25"/>
       <c r="G76" s="6"/>
     </row>
     <row r="77" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B77" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C77" s="25"/>
-      <c r="D77" s="25"/>
-      <c r="E77" s="25"/>
-      <c r="F77" s="25"/>
       <c r="G77" s="6"/>
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B78" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C78" s="25"/>
-      <c r="D78" s="25"/>
-      <c r="E78" s="25"/>
-      <c r="F78" s="25"/>
       <c r="G78" s="6"/>
     </row>
     <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B79" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C79" s="25"/>
-      <c r="D79" s="25"/>
-      <c r="E79" s="25"/>
-      <c r="F79" s="25"/>
       <c r="G79" s="6"/>
     </row>
     <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B80" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C80" s="25"/>
-      <c r="D80" s="25"/>
-      <c r="E80" s="25"/>
-      <c r="F80" s="25"/>
       <c r="G80" s="6"/>
     </row>
     <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B81" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C81" s="25"/>
-      <c r="D81" s="25"/>
-      <c r="E81" s="25"/>
-      <c r="F81" s="25"/>
       <c r="G81" s="6"/>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C82" s="25"/>
-      <c r="D82" s="25"/>
-      <c r="E82" s="25"/>
-      <c r="F82" s="25"/>
       <c r="G82" s="6"/>
     </row>
     <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83" s="5"/>
-      <c r="C83" s="25"/>
-      <c r="D83" s="25"/>
-      <c r="E83" s="25"/>
-      <c r="F83" s="25"/>
       <c r="G83" s="6"/>
     </row>
     <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C84" s="25"/>
-      <c r="D84" s="25"/>
-      <c r="E84" s="25"/>
-      <c r="F84" s="25"/>
       <c r="G84" s="6"/>
     </row>
     <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C85" s="25"/>
-      <c r="D85" s="25"/>
-      <c r="E85" s="25"/>
-      <c r="F85" s="25"/>
       <c r="G85" s="6"/>
     </row>
     <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B86" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C86" s="25"/>
-      <c r="D86" s="25"/>
-      <c r="E86" s="25"/>
-      <c r="F86" s="25"/>
       <c r="G86" s="6"/>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B87" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C87" s="25"/>
-      <c r="D87" s="25"/>
-      <c r="E87" s="25"/>
-      <c r="F87" s="25"/>
       <c r="G87" s="6"/>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B88" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C88" s="25"/>
-      <c r="D88" s="25"/>
-      <c r="E88" s="25"/>
-      <c r="F88" s="25"/>
       <c r="G88" s="6"/>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C89" s="25"/>
-      <c r="D89" s="25"/>
-      <c r="E89" s="25"/>
-      <c r="F89" s="25"/>
       <c r="G89" s="6"/>
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C90" s="25"/>
-      <c r="D90" s="25"/>
-      <c r="E90" s="25"/>
-      <c r="F90" s="25"/>
       <c r="G90" s="6"/>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B91" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C91" s="25"/>
-      <c r="D91" s="25"/>
-      <c r="E91" s="25"/>
-      <c r="F91" s="25"/>
       <c r="G91" s="6"/>
     </row>
     <row r="92" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B92" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C92" s="25"/>
-      <c r="D92" s="25"/>
-      <c r="E92" s="25"/>
-      <c r="F92" s="25"/>
       <c r="G92" s="6"/>
     </row>
     <row r="93" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B93" s="5"/>
-      <c r="C93" s="25"/>
-      <c r="D93" s="25"/>
-      <c r="E93" s="25"/>
-      <c r="F93" s="25"/>
       <c r="G93" s="6"/>
     </row>
     <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B94" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C94" s="25"/>
-      <c r="D94" s="25"/>
-      <c r="E94" s="25"/>
-      <c r="F94" s="25"/>
       <c r="G94" s="6"/>
     </row>
     <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B95" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C95" s="25"/>
-      <c r="D95" s="25"/>
-      <c r="E95" s="25"/>
-      <c r="F95" s="25"/>
       <c r="G95" s="6"/>
     </row>
     <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B96" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C96" s="25"/>
-      <c r="D96" s="25"/>
-      <c r="E96" s="25"/>
-      <c r="F96" s="25"/>
       <c r="G96" s="6"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B97" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C97" s="25"/>
-      <c r="D97" s="25"/>
-      <c r="E97" s="25"/>
-      <c r="F97" s="25"/>
       <c r="G97" s="6"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B98" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C98" s="25"/>
-      <c r="D98" s="25"/>
-      <c r="E98" s="25"/>
-      <c r="F98" s="25"/>
       <c r="G98" s="6"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B99" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C99" s="25"/>
-      <c r="D99" s="25"/>
-      <c r="E99" s="25"/>
-      <c r="F99" s="25"/>
       <c r="G99" s="6"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B100" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C100" s="25"/>
-      <c r="D100" s="25"/>
-      <c r="E100" s="25"/>
-      <c r="F100" s="25"/>
       <c r="G100" s="6"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B101" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C101" s="25"/>
-      <c r="D101" s="25"/>
-      <c r="E101" s="25"/>
-      <c r="F101" s="25"/>
       <c r="G101" s="6"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B102" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C102" s="25"/>
-      <c r="D102" s="25"/>
-      <c r="E102" s="25"/>
-      <c r="F102" s="25"/>
       <c r="G102" s="6"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B103" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C103" s="25"/>
-      <c r="D103" s="25"/>
-      <c r="E103" s="25"/>
-      <c r="F103" s="25"/>
       <c r="G103" s="6"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B104" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C104" s="25"/>
-      <c r="D104" s="25"/>
-      <c r="E104" s="25"/>
-      <c r="F104" s="25"/>
       <c r="G104" s="6"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B105" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C105" s="25"/>
-      <c r="D105" s="25"/>
-      <c r="E105" s="25"/>
-      <c r="F105" s="25"/>
       <c r="G105" s="6"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -3123,96 +3239,56 @@
       <c r="B111" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C111" s="25"/>
-      <c r="D111" s="25"/>
-      <c r="E111" s="25"/>
-      <c r="F111" s="25"/>
       <c r="G111" s="6"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B112" s="5"/>
-      <c r="C112" s="25"/>
-      <c r="D112" s="25"/>
-      <c r="E112" s="25"/>
-      <c r="F112" s="25"/>
       <c r="G112" s="6"/>
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B113" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C113" s="25"/>
-      <c r="D113" s="25"/>
-      <c r="E113" s="25"/>
-      <c r="F113" s="25"/>
       <c r="G113" s="6"/>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B114" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C114" s="25"/>
-      <c r="D114" s="25"/>
-      <c r="E114" s="25"/>
-      <c r="F114" s="25"/>
       <c r="G114" s="6"/>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B115" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C115" s="25"/>
-      <c r="D115" s="25"/>
-      <c r="E115" s="25"/>
-      <c r="F115" s="25"/>
       <c r="G115" s="6"/>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B116" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C116" s="25"/>
-      <c r="D116" s="25"/>
-      <c r="E116" s="25"/>
-      <c r="F116" s="25"/>
       <c r="G116" s="6"/>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B117" s="5"/>
-      <c r="C117" s="25"/>
-      <c r="D117" s="25"/>
-      <c r="E117" s="25"/>
-      <c r="F117" s="25"/>
       <c r="G117" s="6"/>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B118" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C118" s="25"/>
-      <c r="D118" s="25"/>
-      <c r="E118" s="25"/>
-      <c r="F118" s="25"/>
       <c r="G118" s="6"/>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B119" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C119" s="25"/>
-      <c r="D119" s="25"/>
-      <c r="E119" s="25"/>
-      <c r="F119" s="25"/>
       <c r="G119" s="6"/>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B120" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C120" s="25"/>
-      <c r="D120" s="25"/>
-      <c r="E120" s="25"/>
-      <c r="F120" s="25"/>
       <c r="G120" s="6"/>
       <c r="H120" t="s">
         <v>23</v>
@@ -3223,78 +3299,46 @@
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B121" s="14"/>
-      <c r="C121" s="25"/>
-      <c r="D121" s="25"/>
-      <c r="E121" s="25"/>
-      <c r="F121" s="25"/>
       <c r="G121" s="6"/>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B122" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C122" s="25"/>
-      <c r="D122" s="25"/>
-      <c r="E122" s="25"/>
-      <c r="F122" s="25"/>
       <c r="G122" s="6"/>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B123" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="C123" s="25"/>
-      <c r="D123" s="25"/>
-      <c r="E123" s="25"/>
-      <c r="F123" s="25"/>
       <c r="G123" s="6"/>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B124" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C124" s="25"/>
-      <c r="D124" s="25"/>
-      <c r="E124" s="25"/>
-      <c r="F124" s="25"/>
       <c r="G124" s="6"/>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B125" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C125" s="25"/>
-      <c r="D125" s="25"/>
-      <c r="E125" s="25"/>
-      <c r="F125" s="25"/>
       <c r="G125" s="6"/>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B126" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="C126" s="25"/>
-      <c r="D126" s="25"/>
-      <c r="E126" s="25"/>
-      <c r="F126" s="25"/>
       <c r="G126" s="6"/>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B127" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C127" s="25"/>
-      <c r="D127" s="25"/>
-      <c r="E127" s="25"/>
-      <c r="F127" s="25"/>
       <c r="G127" s="6"/>
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B128" s="5"/>
-      <c r="C128" s="25"/>
-      <c r="D128" s="25"/>
-      <c r="E128" s="25"/>
-      <c r="F128" s="25"/>
       <c r="G128" s="6"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -3308,7 +3352,7 @@
       <c r="G129" s="12"/>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="26" t="s">
+      <c r="A132" s="15" t="s">
         <v>94</v>
       </c>
       <c r="B132" s="3"/>
@@ -3322,158 +3366,61 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="5"/>
-      <c r="B133" s="27" t="s">
+      <c r="B133" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C133" s="25"/>
-      <c r="D133" s="25"/>
-      <c r="E133" s="25"/>
-      <c r="F133" s="25"/>
-      <c r="G133" s="25"/>
-      <c r="H133" s="25"/>
       <c r="I133" s="6"/>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="5"/>
-      <c r="B134" s="25"/>
-      <c r="C134" s="25"/>
-      <c r="D134" s="25"/>
-      <c r="E134" s="25"/>
-      <c r="F134" s="25"/>
-      <c r="G134" s="25"/>
-      <c r="H134" s="25"/>
       <c r="I134" s="6"/>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="5"/>
-      <c r="B135" s="25"/>
-      <c r="C135" s="25"/>
-      <c r="D135" s="25"/>
-      <c r="E135" s="25"/>
-      <c r="F135" s="25"/>
-      <c r="G135" s="25"/>
-      <c r="H135" s="25"/>
       <c r="I135" s="6"/>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="5"/>
-      <c r="B136" s="25"/>
-      <c r="C136" s="25"/>
-      <c r="D136" s="25"/>
-      <c r="E136" s="25"/>
-      <c r="F136" s="25"/>
-      <c r="G136" s="25"/>
-      <c r="H136" s="25"/>
       <c r="I136" s="6"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="5"/>
-      <c r="B137" s="25"/>
-      <c r="C137" s="25"/>
-      <c r="D137" s="25"/>
-      <c r="E137" s="25"/>
-      <c r="F137" s="25"/>
-      <c r="G137" s="25"/>
-      <c r="H137" s="25"/>
       <c r="I137" s="6"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="5"/>
-      <c r="B138" s="25"/>
-      <c r="C138" s="25"/>
-      <c r="D138" s="25"/>
-      <c r="E138" s="25"/>
-      <c r="F138" s="25"/>
-      <c r="G138" s="25"/>
-      <c r="H138" s="25"/>
       <c r="I138" s="6"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="5"/>
-      <c r="B139" s="25"/>
-      <c r="C139" s="25"/>
-      <c r="D139" s="25"/>
-      <c r="E139" s="25"/>
-      <c r="F139" s="25"/>
-      <c r="G139" s="25"/>
-      <c r="H139" s="25"/>
       <c r="I139" s="6"/>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="5"/>
-      <c r="B140" s="25"/>
-      <c r="C140" s="25"/>
-      <c r="D140" s="25"/>
-      <c r="E140" s="25"/>
-      <c r="F140" s="25"/>
-      <c r="G140" s="25"/>
-      <c r="H140" s="25"/>
       <c r="I140" s="6"/>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="5"/>
-      <c r="B141" s="25"/>
-      <c r="C141" s="25"/>
-      <c r="D141" s="25"/>
-      <c r="E141" s="25"/>
-      <c r="F141" s="25"/>
-      <c r="G141" s="25"/>
-      <c r="H141" s="25"/>
       <c r="I141" s="6"/>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="5"/>
-      <c r="B142" s="25"/>
-      <c r="C142" s="25"/>
-      <c r="D142" s="25"/>
-      <c r="E142" s="25"/>
-      <c r="F142" s="25"/>
-      <c r="G142" s="25"/>
-      <c r="H142" s="25"/>
       <c r="I142" s="6"/>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="5"/>
-      <c r="B143" s="25"/>
-      <c r="C143" s="25"/>
-      <c r="D143" s="25"/>
-      <c r="E143" s="25"/>
-      <c r="F143" s="25"/>
-      <c r="G143" s="25"/>
-      <c r="H143" s="25"/>
       <c r="I143" s="6"/>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="5"/>
-      <c r="B144" s="25"/>
-      <c r="C144" s="25"/>
-      <c r="D144" s="25"/>
-      <c r="E144" s="25"/>
-      <c r="F144" s="25"/>
-      <c r="G144" s="25"/>
-      <c r="H144" s="25"/>
       <c r="I144" s="6"/>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="5"/>
-      <c r="B145" s="25"/>
-      <c r="C145" s="25"/>
-      <c r="D145" s="25"/>
-      <c r="E145" s="25"/>
-      <c r="F145" s="25"/>
-      <c r="G145" s="25"/>
-      <c r="H145" s="25"/>
       <c r="I145" s="6"/>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="5"/>
-      <c r="B146" s="25"/>
-      <c r="C146" s="25"/>
-      <c r="D146" s="25"/>
-      <c r="E146" s="25"/>
-      <c r="F146" s="25"/>
-      <c r="G146" s="25"/>
-      <c r="H146" s="25"/>
       <c r="I146" s="6"/>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
@@ -3491,4 +3438,1247 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B821525F-6940-4D5F-9FA4-67E6E9566277}">
+  <dimension ref="A2:S226"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="M148" sqref="M148"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="4"/>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="S5" s="6"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+      <c r="S6" s="6"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="S7" s="6"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="S8" s="6"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="S9" s="6"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="S10" s="6"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="S11" s="6"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="S12" s="6"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="S13" s="6"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="S14" s="6"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="S15" s="6"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="S16" s="6"/>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="S17" s="6"/>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="S18" s="6"/>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="S19" s="6"/>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="S20" s="6"/>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="S21" s="6"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="S22" s="6"/>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="S23" s="6"/>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="S24" s="6"/>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="S25" s="6"/>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="S26" s="6"/>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="S27" s="6"/>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="S28" s="6"/>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="S29" s="6"/>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="S30" s="6"/>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="S31" s="6"/>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="S32" s="6"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B33" s="10"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="12"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B38" s="5"/>
+      <c r="C38" t="s">
+        <v>3</v>
+      </c>
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B39" s="5"/>
+      <c r="D39" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" s="6"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B40" s="5"/>
+      <c r="E40" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40" s="6"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B41" s="5"/>
+      <c r="F41" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B42" s="5"/>
+      <c r="E42" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="6"/>
+      <c r="G42" t="s">
+        <v>23</v>
+      </c>
+      <c r="H42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B43" s="5"/>
+      <c r="E43" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" s="6"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B44" s="5"/>
+      <c r="D44" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="6"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B45" s="5"/>
+      <c r="D45" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" s="6"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B46" s="5"/>
+      <c r="E46" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" s="6"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B47" s="5"/>
+      <c r="F47" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B48" s="5"/>
+      <c r="F48" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B49" s="5"/>
+      <c r="C49" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" s="6"/>
+    </row>
+    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B50" s="5"/>
+      <c r="D50" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="6"/>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B51" s="5"/>
+      <c r="D51" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" s="6"/>
+    </row>
+    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B52" s="5"/>
+      <c r="D52" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F52" s="6"/>
+      <c r="G52" t="s">
+        <v>23</v>
+      </c>
+      <c r="H52" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B53" s="5"/>
+      <c r="C53" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53" s="6"/>
+    </row>
+    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B54" s="5"/>
+      <c r="C54" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" s="6"/>
+    </row>
+    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B55" s="5"/>
+      <c r="D55" t="s">
+        <v>16</v>
+      </c>
+      <c r="F55" s="6"/>
+    </row>
+    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B56" s="5"/>
+      <c r="D56" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F56" s="6"/>
+      <c r="G56" t="s">
+        <v>23</v>
+      </c>
+      <c r="H56" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B57" s="10"/>
+      <c r="C57" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="12"/>
+    </row>
+    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="4"/>
+    </row>
+    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B61" s="5"/>
+      <c r="N61" s="6"/>
+    </row>
+    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B62" s="5"/>
+      <c r="N62" s="6"/>
+    </row>
+    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B63" s="5"/>
+      <c r="N63" s="6"/>
+    </row>
+    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B64" s="5"/>
+      <c r="N64" s="6"/>
+    </row>
+    <row r="65" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B65" s="5"/>
+      <c r="N65" s="6"/>
+    </row>
+    <row r="66" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B66" s="5"/>
+      <c r="N66" s="6"/>
+    </row>
+    <row r="67" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B67" s="5"/>
+      <c r="N67" s="6"/>
+    </row>
+    <row r="68" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B68" s="5"/>
+      <c r="N68" s="6"/>
+    </row>
+    <row r="69" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B69" s="5"/>
+      <c r="N69" s="6"/>
+    </row>
+    <row r="70" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B70" s="5"/>
+      <c r="N70" s="6"/>
+    </row>
+    <row r="71" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B71" s="5"/>
+      <c r="N71" s="6"/>
+    </row>
+    <row r="72" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B72" s="5"/>
+      <c r="N72" s="6"/>
+    </row>
+    <row r="73" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B73" s="5"/>
+      <c r="N73" s="6"/>
+    </row>
+    <row r="74" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B74" s="5"/>
+      <c r="N74" s="6"/>
+    </row>
+    <row r="75" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B75" s="5"/>
+      <c r="N75" s="6"/>
+    </row>
+    <row r="76" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B76" s="5"/>
+      <c r="N76" s="6"/>
+    </row>
+    <row r="77" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B77" s="5"/>
+      <c r="N77" s="6"/>
+    </row>
+    <row r="78" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B78" s="5"/>
+      <c r="N78" s="6"/>
+    </row>
+    <row r="79" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B79" s="5"/>
+      <c r="N79" s="6"/>
+    </row>
+    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B80" s="5"/>
+      <c r="N80" s="6"/>
+    </row>
+    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B81" s="5"/>
+      <c r="N81" s="6"/>
+    </row>
+    <row r="82" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B82" s="5"/>
+      <c r="N82" s="6"/>
+    </row>
+    <row r="83" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B83" s="5"/>
+      <c r="N83" s="6"/>
+    </row>
+    <row r="84" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B84" s="5"/>
+      <c r="N84" s="6"/>
+    </row>
+    <row r="85" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B85" s="5"/>
+      <c r="N85" s="6"/>
+    </row>
+    <row r="86" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B86" s="5"/>
+      <c r="N86" s="6"/>
+    </row>
+    <row r="87" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B87" s="5"/>
+      <c r="N87" s="6"/>
+    </row>
+    <row r="88" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B88" s="5"/>
+      <c r="N88" s="6"/>
+    </row>
+    <row r="89" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B89" s="5"/>
+      <c r="N89" s="6"/>
+    </row>
+    <row r="90" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B90" s="5"/>
+      <c r="N90" s="6"/>
+    </row>
+    <row r="91" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B91" s="5"/>
+      <c r="N91" s="6"/>
+    </row>
+    <row r="92" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B92" s="5"/>
+      <c r="N92" s="6"/>
+    </row>
+    <row r="93" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B93" s="5"/>
+      <c r="N93" s="6"/>
+    </row>
+    <row r="94" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B94" s="5"/>
+      <c r="N94" s="6"/>
+    </row>
+    <row r="95" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B95" s="5"/>
+      <c r="N95" s="6"/>
+    </row>
+    <row r="96" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B96" s="5"/>
+      <c r="N96" s="6"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B97" s="5"/>
+      <c r="N97" s="6"/>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B98" s="5"/>
+      <c r="N98" s="6"/>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B99" s="5"/>
+      <c r="N99" s="6"/>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B100" s="5"/>
+      <c r="N100" s="6"/>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B101" s="5"/>
+      <c r="N101" s="6"/>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B102" s="5"/>
+      <c r="N102" s="6"/>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B103" s="5"/>
+      <c r="N103" s="6"/>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B104" s="10"/>
+      <c r="C104" s="11"/>
+      <c r="D104" s="11"/>
+      <c r="E104" s="11"/>
+      <c r="F104" s="11"/>
+      <c r="G104" s="11"/>
+      <c r="H104" s="11"/>
+      <c r="I104" s="11"/>
+      <c r="J104" s="11"/>
+      <c r="K104" s="11"/>
+      <c r="L104" s="11"/>
+      <c r="M104" s="11"/>
+      <c r="N104" s="12"/>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B108" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="3"/>
+      <c r="F108" s="3"/>
+      <c r="G108" s="3"/>
+      <c r="H108" s="3"/>
+      <c r="I108" s="3"/>
+      <c r="J108" s="4"/>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B109" s="5"/>
+      <c r="J109" s="6"/>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B110" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J110" s="6"/>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B111" s="5"/>
+      <c r="J111" s="6"/>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B112" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J112" s="6"/>
+    </row>
+    <row r="113" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B113" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J113" s="6"/>
+    </row>
+    <row r="114" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B114" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J114" s="6"/>
+    </row>
+    <row r="115" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B115" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J115" s="6"/>
+    </row>
+    <row r="116" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B116" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J116" s="6"/>
+    </row>
+    <row r="117" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B117" s="5"/>
+      <c r="J117" s="6"/>
+    </row>
+    <row r="118" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B118" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J118" s="6"/>
+    </row>
+    <row r="119" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B119" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J119" s="6"/>
+    </row>
+    <row r="120" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B120" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J120" s="6"/>
+    </row>
+    <row r="121" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B121" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J121" s="6"/>
+    </row>
+    <row r="122" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B122" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J122" s="6"/>
+    </row>
+    <row r="123" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B123" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J123" s="6"/>
+    </row>
+    <row r="124" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B124" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J124" s="6"/>
+    </row>
+    <row r="125" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B125" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="J125" s="6"/>
+    </row>
+    <row r="126" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B126" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J126" s="6"/>
+    </row>
+    <row r="127" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B127" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J127" s="6"/>
+    </row>
+    <row r="128" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B128" s="5"/>
+      <c r="J128" s="6"/>
+    </row>
+    <row r="129" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B129" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J129" s="6"/>
+    </row>
+    <row r="130" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B130" s="5"/>
+      <c r="J130" s="6"/>
+    </row>
+    <row r="131" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B131" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J131" s="6"/>
+    </row>
+    <row r="132" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B132" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J132" s="6"/>
+    </row>
+    <row r="133" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B133" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J133" s="6"/>
+    </row>
+    <row r="134" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B134" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J134" s="6"/>
+    </row>
+    <row r="135" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B135" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J135" s="6"/>
+    </row>
+    <row r="136" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B136" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J136" s="6"/>
+    </row>
+    <row r="137" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B137" s="5"/>
+      <c r="J137" s="6"/>
+    </row>
+    <row r="138" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B138" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="J138" s="6"/>
+    </row>
+    <row r="139" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B139" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="J139" s="6"/>
+    </row>
+    <row r="140" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B140" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="J140" s="6"/>
+    </row>
+    <row r="141" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B141" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="J141" s="6"/>
+    </row>
+    <row r="142" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B142" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="J142" s="6"/>
+    </row>
+    <row r="143" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B143" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="J143" s="6"/>
+    </row>
+    <row r="144" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B144" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J144" s="6"/>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B145" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="J145" s="6"/>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B146" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="J146" s="6"/>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B147" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J147" s="6"/>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B148" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="J148" s="6"/>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B149" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="J149" s="6"/>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B150" s="14"/>
+      <c r="J150" s="6"/>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B151" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="J151" s="6"/>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B152" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J152" s="6"/>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B153" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C153" s="11"/>
+      <c r="D153" s="11"/>
+      <c r="E153" s="11"/>
+      <c r="F153" s="11"/>
+      <c r="G153" s="11"/>
+      <c r="H153" s="11"/>
+      <c r="I153" s="11"/>
+      <c r="J153" s="12"/>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B157" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C157" s="3"/>
+      <c r="D157" s="3"/>
+      <c r="E157" s="3"/>
+      <c r="F157" s="3"/>
+      <c r="G157" s="4"/>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B158" s="5"/>
+      <c r="G158" s="6"/>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B159" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G159" s="6"/>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B160" s="5"/>
+      <c r="G160" s="6"/>
+    </row>
+    <row r="161" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B161" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G161" s="6"/>
+    </row>
+    <row r="162" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B162" s="5"/>
+      <c r="G162" s="6"/>
+    </row>
+    <row r="163" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B163" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G163" s="6"/>
+    </row>
+    <row r="164" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B164" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G164" s="6"/>
+    </row>
+    <row r="165" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B165" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G165" s="6"/>
+    </row>
+    <row r="166" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B166" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G166" s="6"/>
+    </row>
+    <row r="167" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B167" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G167" s="6"/>
+    </row>
+    <row r="168" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B168" s="5"/>
+      <c r="G168" s="6"/>
+    </row>
+    <row r="169" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B169" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G169" s="6"/>
+    </row>
+    <row r="170" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B170" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G170" s="6"/>
+    </row>
+    <row r="171" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B171" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G171" s="6"/>
+    </row>
+    <row r="172" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B172" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G172" s="6"/>
+    </row>
+    <row r="173" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B173" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G173" s="6"/>
+    </row>
+    <row r="174" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B174" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G174" s="6"/>
+    </row>
+    <row r="175" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B175" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G175" s="6"/>
+    </row>
+    <row r="176" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B176" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G176" s="6"/>
+    </row>
+    <row r="177" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B177" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G177" s="6"/>
+    </row>
+    <row r="178" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B178" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G178" s="6"/>
+    </row>
+    <row r="179" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B179" s="5"/>
+      <c r="G179" s="6"/>
+    </row>
+    <row r="180" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B180" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G180" s="6"/>
+    </row>
+    <row r="181" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B181" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G181" s="6"/>
+    </row>
+    <row r="182" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B182" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G182" s="6"/>
+    </row>
+    <row r="183" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B183" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G183" s="6"/>
+    </row>
+    <row r="184" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B184" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G184" s="6"/>
+    </row>
+    <row r="185" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B185" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G185" s="6"/>
+    </row>
+    <row r="186" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B186" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G186" s="6"/>
+    </row>
+    <row r="187" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B187" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G187" s="6"/>
+    </row>
+    <row r="188" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B188" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G188" s="6"/>
+    </row>
+    <row r="189" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B189" s="5"/>
+      <c r="G189" s="6"/>
+    </row>
+    <row r="190" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B190" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G190" s="6"/>
+    </row>
+    <row r="191" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B191" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G191" s="6"/>
+    </row>
+    <row r="192" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B192" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G192" s="6"/>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B193" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G193" s="6"/>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B194" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G194" s="6"/>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B195" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G195" s="6"/>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B196" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G196" s="6"/>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B197" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="G197" s="6"/>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B198" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G198" s="6"/>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B199" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G199" s="6"/>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B200" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G200" s="6"/>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B201" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G201" s="6"/>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B202" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C202" s="11"/>
+      <c r="D202" s="11"/>
+      <c r="E202" s="11"/>
+      <c r="F202" s="11"/>
+      <c r="G202" s="12"/>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B206" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C206" s="3"/>
+      <c r="D206" s="3"/>
+      <c r="E206" s="3"/>
+      <c r="F206" s="3"/>
+      <c r="G206" s="4"/>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B207" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G207" s="6"/>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B208" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G208" s="6"/>
+    </row>
+    <row r="209" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B209" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G209" s="6"/>
+    </row>
+    <row r="210" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B210" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G210" s="6"/>
+    </row>
+    <row r="211" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B211" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G211" s="6"/>
+    </row>
+    <row r="212" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B212" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G212" s="6"/>
+    </row>
+    <row r="213" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B213" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G213" s="6"/>
+    </row>
+    <row r="214" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B214" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G214" s="6"/>
+    </row>
+    <row r="215" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B215" s="5"/>
+      <c r="G215" s="6"/>
+    </row>
+    <row r="216" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B216" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G216" s="6"/>
+    </row>
+    <row r="217" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B217" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G217" s="6"/>
+    </row>
+    <row r="218" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B218" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G218" s="6"/>
+    </row>
+    <row r="219" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B219" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G219" s="6"/>
+    </row>
+    <row r="220" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B220" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G220" s="6"/>
+    </row>
+    <row r="221" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B221" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G221" s="6"/>
+    </row>
+    <row r="222" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B222" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C222" s="11"/>
+      <c r="D222" s="11"/>
+      <c r="E222" s="11"/>
+      <c r="F222" s="11"/>
+      <c r="G222" s="12"/>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B226" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Remove repetition in the view templates: add a base template to inherit from
</commit_message>
<xml_diff>
--- a/me/4.Views.xlsx
+++ b/me/4.Views.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\build-php-mvc-framework\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F57235C-AEC2-45AA-AF5D-E59AC0358C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E33A7CC-D33D-464A-8318-E1E85A539E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Display a view" sheetId="1" r:id="rId1"/>
     <sheet name="PassDataFromControllerToView" sheetId="2" r:id="rId2"/>
     <sheet name="add a template engine" sheetId="3" r:id="rId3"/>
+    <sheet name="add a base template" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="157">
   <si>
     <t>Display a view: create a class to render views and use it in a controller</t>
   </si>
@@ -519,6 +520,105 @@
   </si>
   <si>
     <t>        echo $twig-&gt;render($template, $args);</t>
+  </si>
+  <si>
+    <t>Remove repetition in the view templates: add a base template to inherit from</t>
+  </si>
+  <si>
+    <t>base.html</t>
+  </si>
+  <si>
+    <t>build-php-mvc-framework\App\Views\base.html</t>
+  </si>
+  <si>
+    <t>    &lt;title&gt;{% block title %}{% endblock %}&lt;/title&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;nav&gt;</t>
+  </si>
+  <si>
+    <t>        &lt;a href="/"&gt;Home&lt;/a&gt; |</t>
+  </si>
+  <si>
+    <t>        &lt;a href="/posts/index"&gt;Posts&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;/nav&gt;</t>
+  </si>
+  <si>
+    <t>    {% block body %}</t>
+  </si>
+  <si>
+    <t>    {% endblock %}</t>
+  </si>
+  <si>
+    <t>{% extends "base.html" %}</t>
+  </si>
+  <si>
+    <t>{% block title %}Home{% endblock %}</t>
+  </si>
+  <si>
+    <t>{% block body %}</t>
+  </si>
+  <si>
+    <t>    &lt;p&gt;Hello from a Twig template, {{ name }}!&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>            &lt;li&gt;{{ colour }}&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>{% endblock %}</t>
+  </si>
+  <si>
+    <t>build-php-mvc-framework\App\Controllers\Posts.php</t>
+  </si>
+  <si>
+    <t> * Posts controller</t>
+  </si>
+  <si>
+    <t> *</t>
+  </si>
+  <si>
+    <t>class Posts extends \Core\Controller</t>
+  </si>
+  <si>
+    <t>        View::renderTemplate('Posts/index.html');</t>
+  </si>
+  <si>
+    <t>     * Show the add new page</t>
+  </si>
+  <si>
+    <t>    public function addNewAction()</t>
+  </si>
+  <si>
+    <t>        echo 'Hello from the addNew action in the Posts controller!';</t>
+  </si>
+  <si>
+    <t>     * Show the edit page</t>
+  </si>
+  <si>
+    <t>    public function editAction()</t>
+  </si>
+  <si>
+    <t>        echo 'Hello from the edit action in the Posts controller!';</t>
+  </si>
+  <si>
+    <t>        echo '&lt;p&gt;Route parameters: &lt;pre&gt;' .</t>
+  </si>
+  <si>
+    <t>            htmlspecialchars(print_r($this-&gt;route_params, true)) . '&lt;/pre&gt;&lt;/p&gt;';</t>
+  </si>
+  <si>
+    <t>build-php-mvc-framework\App\Views\Posts\index.html</t>
+  </si>
+  <si>
+    <t>{% block title %}Posts{% endblock %}</t>
+  </si>
+  <si>
+    <t>    &lt;h1&gt;Posts&lt;/h1&gt;</t>
+  </si>
+  <si>
+    <t>Sau khi click thì redirect sang trang http://localhost/posts/index</t>
   </si>
 </sst>
 </file>
@@ -647,7 +747,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -665,7 +765,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1571,6 +1683,405 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>323849</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>17249</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E54BE44-160C-1E04-9DA7-133DF9236085}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685799" y="666750"/>
+          <a:ext cx="10791825" cy="5446499"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D340492-BABA-CBA3-EADD-DCAFA32C7E9D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1371600" y="12363450"/>
+          <a:ext cx="361950" cy="3181350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03643145-CBC1-1316-3BF8-A62A7E086EC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1181100" y="13896975"/>
+          <a:ext cx="142875" cy="1962150"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38145DE8-E5D0-C1AF-DB6F-C738F7FB30F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1619250" y="11401425"/>
+          <a:ext cx="838200" cy="3724275"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>503343</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>151946</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4EA0CD1-E167-5A56-8EDC-6CB1B04BA310}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5286375" y="19383375"/>
+          <a:ext cx="11857143" cy="3628571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>580404</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>85387</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD78387B-38F3-D1CF-7E98-C26D6FE79A79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="666750" y="30337125"/>
+          <a:ext cx="4971429" cy="2704762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>176</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>752090</xdr:colOff>
+      <xdr:row>185</xdr:row>
+      <xdr:rowOff>104556</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D7D1848-354F-EAD4-3F5A-14C11B8F4F10}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723900" y="33594675"/>
+          <a:ext cx="3076190" cy="1752381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>175</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32A2FD0C-A0F9-A88C-F7B8-FCCA1A0AF100}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1276350" y="31308675"/>
+          <a:ext cx="104775" cy="2057400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3444,8 +3955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B821525F-6940-4D5F-9FA4-67E6E9566277}">
   <dimension ref="A2:S226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="M148" sqref="M148"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4514,7 +5025,7 @@
       <c r="G196" s="6"/>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B197" s="17" t="s">
+      <c r="B197" s="5" t="s">
         <v>121</v>
       </c>
       <c r="G197" s="6"/>
@@ -4681,4 +5192,1461 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CC6748E-DA62-4AB5-B3DB-30AFF5879A13}">
+  <dimension ref="A2:J186"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="M154" sqref="M154"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="18"/>
+      <c r="B36" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="21"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="18"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="23"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="18"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" s="18"/>
+      <c r="F38" s="23"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="18"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F39" s="23"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="18"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="18"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="23"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="18"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="23"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="18"/>
+      <c r="F43" s="23"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="18"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="18"/>
+      <c r="F44" s="23"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="18"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" s="23"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="18"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="18"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="H47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="18"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="F48" s="23"/>
+      <c r="H48" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="18"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="23"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="18"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" s="18"/>
+      <c r="F50" s="23"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="18"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51" s="18"/>
+      <c r="F51" s="23"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="18"/>
+      <c r="B52" s="22"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E52" s="18"/>
+      <c r="F52" s="23"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="18"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="23"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="18"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="23"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="18"/>
+      <c r="B55" s="22"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E55" s="18"/>
+      <c r="F55" s="23"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="18"/>
+      <c r="B56" s="22"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56" s="18"/>
+      <c r="F56" s="23"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="18"/>
+      <c r="B57" s="25"/>
+      <c r="C57" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="27"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="4"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62" s="28"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="28"/>
+      <c r="F62" s="6"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63" s="28"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="28"/>
+      <c r="F63" s="6"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64" s="28"/>
+      <c r="D64" s="28"/>
+      <c r="E64" s="28"/>
+      <c r="F64" s="6"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B65" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C65" s="28"/>
+      <c r="D65" s="28"/>
+      <c r="E65" s="28"/>
+      <c r="F65" s="6"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B66" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" s="28"/>
+      <c r="D66" s="28"/>
+      <c r="E66" s="28"/>
+      <c r="F66" s="6"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C67" s="28"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="28"/>
+      <c r="F67" s="6"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B68" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C68" s="28"/>
+      <c r="D68" s="28"/>
+      <c r="E68" s="28"/>
+      <c r="F68" s="6"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B69" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C69" s="28"/>
+      <c r="D69" s="28"/>
+      <c r="E69" s="28"/>
+      <c r="F69" s="6"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B70" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C70" s="28"/>
+      <c r="D70" s="28"/>
+      <c r="E70" s="28"/>
+      <c r="F70" s="6"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B71" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C71" s="28"/>
+      <c r="D71" s="28"/>
+      <c r="E71" s="28"/>
+      <c r="F71" s="6"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B72" s="5"/>
+      <c r="C72" s="28"/>
+      <c r="D72" s="28"/>
+      <c r="E72" s="28"/>
+      <c r="F72" s="6"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B73" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C73" s="28"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="28"/>
+      <c r="F73" s="6"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B74" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C74" s="28"/>
+      <c r="D74" s="28"/>
+      <c r="E74" s="28"/>
+      <c r="F74" s="6"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B75" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C75" s="28"/>
+      <c r="D75" s="28"/>
+      <c r="E75" s="28"/>
+      <c r="F75" s="6"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B76" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="12"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B80" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="4"/>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B81" s="5"/>
+      <c r="C81" s="28"/>
+      <c r="D81" s="28"/>
+      <c r="E81" s="28"/>
+      <c r="F81" s="6"/>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B82" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C82" s="28"/>
+      <c r="D82" s="28"/>
+      <c r="E82" s="28"/>
+      <c r="F82" s="6"/>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B83" s="5"/>
+      <c r="C83" s="28"/>
+      <c r="D83" s="28"/>
+      <c r="E83" s="28"/>
+      <c r="F83" s="6"/>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B84" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C84" s="28"/>
+      <c r="D84" s="28"/>
+      <c r="E84" s="28"/>
+      <c r="F84" s="6"/>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B85" s="5"/>
+      <c r="C85" s="28"/>
+      <c r="D85" s="28"/>
+      <c r="E85" s="28"/>
+      <c r="F85" s="6"/>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B86" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C86" s="28"/>
+      <c r="D86" s="28"/>
+      <c r="E86" s="28"/>
+      <c r="F86" s="6"/>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B87" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C87" s="28"/>
+      <c r="D87" s="28"/>
+      <c r="E87" s="28"/>
+      <c r="F87" s="6"/>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B88" s="5"/>
+      <c r="C88" s="28"/>
+      <c r="D88" s="28"/>
+      <c r="E88" s="28"/>
+      <c r="F88" s="6"/>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B89" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C89" s="28"/>
+      <c r="D89" s="28"/>
+      <c r="E89" s="28"/>
+      <c r="F89" s="6"/>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B90" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C90" s="28"/>
+      <c r="D90" s="28"/>
+      <c r="E90" s="28"/>
+      <c r="F90" s="6"/>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B91" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C91" s="28"/>
+      <c r="D91" s="28"/>
+      <c r="E91" s="28"/>
+      <c r="F91" s="6"/>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B92" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C92" s="28"/>
+      <c r="D92" s="28"/>
+      <c r="E92" s="28"/>
+      <c r="F92" s="6"/>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B93" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C93" s="28"/>
+      <c r="D93" s="28"/>
+      <c r="E93" s="28"/>
+      <c r="F93" s="6"/>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B94" s="5"/>
+      <c r="C94" s="28"/>
+      <c r="D94" s="28"/>
+      <c r="E94" s="28"/>
+      <c r="F94" s="6"/>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B95" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C95" s="11"/>
+      <c r="D95" s="11"/>
+      <c r="E95" s="11"/>
+      <c r="F95" s="12"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B99" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3"/>
+      <c r="G99" s="3"/>
+      <c r="H99" s="4"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B100" s="5"/>
+      <c r="C100" s="28"/>
+      <c r="D100" s="28"/>
+      <c r="E100" s="28"/>
+      <c r="F100" s="28"/>
+      <c r="G100" s="28"/>
+      <c r="H100" s="6"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B101" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C101" s="28"/>
+      <c r="D101" s="28"/>
+      <c r="E101" s="28"/>
+      <c r="F101" s="28"/>
+      <c r="G101" s="28"/>
+      <c r="H101" s="6"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B102" s="5"/>
+      <c r="C102" s="28"/>
+      <c r="D102" s="28"/>
+      <c r="E102" s="28"/>
+      <c r="F102" s="28"/>
+      <c r="G102" s="28"/>
+      <c r="H102" s="6"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B103" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C103" s="28"/>
+      <c r="D103" s="28"/>
+      <c r="E103" s="28"/>
+      <c r="F103" s="28"/>
+      <c r="G103" s="28"/>
+      <c r="H103" s="6"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B104" s="5"/>
+      <c r="C104" s="28"/>
+      <c r="D104" s="28"/>
+      <c r="E104" s="28"/>
+      <c r="F104" s="28"/>
+      <c r="G104" s="28"/>
+      <c r="H104" s="6"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B105" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C105" s="28"/>
+      <c r="D105" s="28"/>
+      <c r="E105" s="28"/>
+      <c r="F105" s="28"/>
+      <c r="G105" s="28"/>
+      <c r="H105" s="6"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B106" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C106" s="28"/>
+      <c r="D106" s="28"/>
+      <c r="E106" s="28"/>
+      <c r="F106" s="28"/>
+      <c r="G106" s="28"/>
+      <c r="H106" s="6"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B107" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C107" s="28"/>
+      <c r="D107" s="28"/>
+      <c r="E107" s="28"/>
+      <c r="F107" s="28"/>
+      <c r="G107" s="28"/>
+      <c r="H107" s="6"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B108" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C108" s="28"/>
+      <c r="D108" s="28"/>
+      <c r="E108" s="28"/>
+      <c r="F108" s="28"/>
+      <c r="G108" s="28"/>
+      <c r="H108" s="6"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B109" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C109" s="28"/>
+      <c r="D109" s="28"/>
+      <c r="E109" s="28"/>
+      <c r="F109" s="28"/>
+      <c r="G109" s="28"/>
+      <c r="H109" s="6"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B110" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C110" s="28"/>
+      <c r="D110" s="28"/>
+      <c r="E110" s="28"/>
+      <c r="F110" s="28"/>
+      <c r="G110" s="28"/>
+      <c r="H110" s="6"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B111" s="5"/>
+      <c r="C111" s="28"/>
+      <c r="D111" s="28"/>
+      <c r="E111" s="28"/>
+      <c r="F111" s="28"/>
+      <c r="G111" s="28"/>
+      <c r="H111" s="6"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B112" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C112" s="28"/>
+      <c r="D112" s="28"/>
+      <c r="E112" s="28"/>
+      <c r="F112" s="28"/>
+      <c r="G112" s="28"/>
+      <c r="H112" s="6"/>
+    </row>
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B113" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C113" s="28"/>
+      <c r="D113" s="28"/>
+      <c r="E113" s="28"/>
+      <c r="F113" s="28"/>
+      <c r="G113" s="28"/>
+      <c r="H113" s="6"/>
+    </row>
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B114" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C114" s="28"/>
+      <c r="D114" s="28"/>
+      <c r="E114" s="28"/>
+      <c r="F114" s="28"/>
+      <c r="G114" s="28"/>
+      <c r="H114" s="6"/>
+    </row>
+    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B115" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C115" s="28"/>
+      <c r="D115" s="28"/>
+      <c r="E115" s="28"/>
+      <c r="F115" s="28"/>
+      <c r="G115" s="28"/>
+      <c r="H115" s="6"/>
+    </row>
+    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B116" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C116" s="28"/>
+      <c r="D116" s="28"/>
+      <c r="E116" s="28"/>
+      <c r="F116" s="28"/>
+      <c r="G116" s="28"/>
+      <c r="H116" s="6"/>
+    </row>
+    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B117" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C117" s="28"/>
+      <c r="D117" s="28"/>
+      <c r="E117" s="28"/>
+      <c r="F117" s="28"/>
+      <c r="G117" s="28"/>
+      <c r="H117" s="6"/>
+    </row>
+    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B118" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C118" s="28"/>
+      <c r="D118" s="28"/>
+      <c r="E118" s="28"/>
+      <c r="F118" s="28"/>
+      <c r="G118" s="28"/>
+      <c r="H118" s="6"/>
+    </row>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B119" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="C119" s="28"/>
+      <c r="D119" s="28"/>
+      <c r="E119" s="28"/>
+      <c r="F119" s="28"/>
+      <c r="G119" s="28"/>
+      <c r="H119" s="6"/>
+    </row>
+    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B120" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C120" s="28"/>
+      <c r="D120" s="28"/>
+      <c r="E120" s="28"/>
+      <c r="F120" s="28"/>
+      <c r="G120" s="28"/>
+      <c r="H120" s="6"/>
+    </row>
+    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B121" s="5"/>
+      <c r="C121" s="28"/>
+      <c r="D121" s="28"/>
+      <c r="E121" s="28"/>
+      <c r="F121" s="28"/>
+      <c r="G121" s="28"/>
+      <c r="H121" s="6"/>
+    </row>
+    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B122" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C122" s="28"/>
+      <c r="D122" s="28"/>
+      <c r="E122" s="28"/>
+      <c r="F122" s="28"/>
+      <c r="G122" s="28"/>
+      <c r="H122" s="6"/>
+    </row>
+    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B123" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C123" s="28"/>
+      <c r="D123" s="28"/>
+      <c r="E123" s="28"/>
+      <c r="F123" s="28"/>
+      <c r="G123" s="28"/>
+      <c r="H123" s="6"/>
+    </row>
+    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B124" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C124" s="28"/>
+      <c r="D124" s="28"/>
+      <c r="E124" s="28"/>
+      <c r="F124" s="28"/>
+      <c r="G124" s="28"/>
+      <c r="H124" s="6"/>
+    </row>
+    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B125" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C125" s="28"/>
+      <c r="D125" s="28"/>
+      <c r="E125" s="28"/>
+      <c r="F125" s="28"/>
+      <c r="G125" s="28"/>
+      <c r="H125" s="6"/>
+    </row>
+    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B126" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C126" s="28"/>
+      <c r="D126" s="28"/>
+      <c r="E126" s="28"/>
+      <c r="F126" s="28"/>
+      <c r="G126" s="28"/>
+      <c r="H126" s="6"/>
+    </row>
+    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B127" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C127" s="28"/>
+      <c r="D127" s="28"/>
+      <c r="E127" s="28"/>
+      <c r="F127" s="28"/>
+      <c r="G127" s="28"/>
+      <c r="H127" s="6"/>
+    </row>
+    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B128" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C128" s="28"/>
+      <c r="D128" s="28"/>
+      <c r="E128" s="28"/>
+      <c r="F128" s="28"/>
+      <c r="G128" s="28"/>
+      <c r="H128" s="6"/>
+    </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B129" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C129" s="28"/>
+      <c r="D129" s="28"/>
+      <c r="E129" s="28"/>
+      <c r="F129" s="28"/>
+      <c r="G129" s="28"/>
+      <c r="H129" s="6"/>
+    </row>
+    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B130" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C130" s="28"/>
+      <c r="D130" s="28"/>
+      <c r="E130" s="28"/>
+      <c r="F130" s="28"/>
+      <c r="G130" s="28"/>
+      <c r="H130" s="6"/>
+    </row>
+    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B131" s="5"/>
+      <c r="C131" s="28"/>
+      <c r="D131" s="28"/>
+      <c r="E131" s="28"/>
+      <c r="F131" s="28"/>
+      <c r="G131" s="28"/>
+      <c r="H131" s="6"/>
+    </row>
+    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B132" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C132" s="28"/>
+      <c r="D132" s="28"/>
+      <c r="E132" s="28"/>
+      <c r="F132" s="28"/>
+      <c r="G132" s="28"/>
+      <c r="H132" s="6"/>
+    </row>
+    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B133" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C133" s="28"/>
+      <c r="D133" s="28"/>
+      <c r="E133" s="28"/>
+      <c r="F133" s="28"/>
+      <c r="G133" s="28"/>
+      <c r="H133" s="6"/>
+    </row>
+    <row r="134" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B134" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C134" s="28"/>
+      <c r="D134" s="28"/>
+      <c r="E134" s="28"/>
+      <c r="F134" s="28"/>
+      <c r="G134" s="28"/>
+      <c r="H134" s="6"/>
+    </row>
+    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B135" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C135" s="28"/>
+      <c r="D135" s="28"/>
+      <c r="E135" s="28"/>
+      <c r="F135" s="28"/>
+      <c r="G135" s="28"/>
+      <c r="H135" s="6"/>
+    </row>
+    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B136" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C136" s="28"/>
+      <c r="D136" s="28"/>
+      <c r="E136" s="28"/>
+      <c r="F136" s="28"/>
+      <c r="G136" s="28"/>
+      <c r="H136" s="6"/>
+    </row>
+    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B137" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C137" s="28"/>
+      <c r="D137" s="28"/>
+      <c r="E137" s="28"/>
+      <c r="F137" s="28"/>
+      <c r="G137" s="28"/>
+      <c r="H137" s="6"/>
+    </row>
+    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B138" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C138" s="28"/>
+      <c r="D138" s="28"/>
+      <c r="E138" s="28"/>
+      <c r="F138" s="28"/>
+      <c r="G138" s="28"/>
+      <c r="H138" s="6"/>
+    </row>
+    <row r="139" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B139" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C139" s="28"/>
+      <c r="D139" s="28"/>
+      <c r="E139" s="28"/>
+      <c r="F139" s="28"/>
+      <c r="G139" s="28"/>
+      <c r="H139" s="6"/>
+    </row>
+    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B140" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C140" s="28"/>
+      <c r="D140" s="28"/>
+      <c r="E140" s="28"/>
+      <c r="F140" s="28"/>
+      <c r="G140" s="28"/>
+      <c r="H140" s="6"/>
+    </row>
+    <row r="141" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B141" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C141" s="28"/>
+      <c r="D141" s="28"/>
+      <c r="E141" s="28"/>
+      <c r="F141" s="28"/>
+      <c r="G141" s="28"/>
+      <c r="H141" s="6"/>
+    </row>
+    <row r="142" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B142" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C142" s="28"/>
+      <c r="D142" s="28"/>
+      <c r="E142" s="28"/>
+      <c r="F142" s="28"/>
+      <c r="G142" s="28"/>
+      <c r="H142" s="6"/>
+    </row>
+    <row r="143" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B143" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C143" s="11"/>
+      <c r="D143" s="11"/>
+      <c r="E143" s="11"/>
+      <c r="F143" s="11"/>
+      <c r="G143" s="11"/>
+      <c r="H143" s="12"/>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B147" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C147" s="3"/>
+      <c r="D147" s="3"/>
+      <c r="E147" s="4"/>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B148" s="5"/>
+      <c r="C148" s="28"/>
+      <c r="D148" s="28"/>
+      <c r="E148" s="6"/>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B149" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C149" s="28"/>
+      <c r="D149" s="28"/>
+      <c r="E149" s="6"/>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B150" s="5"/>
+      <c r="C150" s="28"/>
+      <c r="D150" s="28"/>
+      <c r="E150" s="6"/>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B151" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C151" s="28"/>
+      <c r="D151" s="28"/>
+      <c r="E151" s="6"/>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B152" s="5"/>
+      <c r="C152" s="28"/>
+      <c r="D152" s="28"/>
+      <c r="E152" s="6"/>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B153" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C153" s="28"/>
+      <c r="D153" s="28"/>
+      <c r="E153" s="6"/>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B154" s="5"/>
+      <c r="C154" s="28"/>
+      <c r="D154" s="28"/>
+      <c r="E154" s="6"/>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B155" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C155" s="11"/>
+      <c r="D155" s="11"/>
+      <c r="E155" s="12"/>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A158" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B158" s="3"/>
+      <c r="C158" s="3"/>
+      <c r="D158" s="3"/>
+      <c r="E158" s="3"/>
+      <c r="F158" s="3"/>
+      <c r="G158" s="3"/>
+      <c r="H158" s="3"/>
+      <c r="I158" s="3"/>
+      <c r="J158" s="4"/>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A159" s="5"/>
+      <c r="B159" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C159" s="28"/>
+      <c r="D159" s="28"/>
+      <c r="E159" s="28"/>
+      <c r="F159" s="28"/>
+      <c r="G159" s="28"/>
+      <c r="H159" s="28"/>
+      <c r="I159" s="28"/>
+      <c r="J159" s="6"/>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A160" s="5"/>
+      <c r="B160" s="28"/>
+      <c r="C160" s="28"/>
+      <c r="D160" s="28"/>
+      <c r="E160" s="28"/>
+      <c r="F160" s="28"/>
+      <c r="G160" s="28"/>
+      <c r="H160" s="28"/>
+      <c r="I160" s="28"/>
+      <c r="J160" s="6"/>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A161" s="5"/>
+      <c r="B161" s="28"/>
+      <c r="C161" s="28"/>
+      <c r="D161" s="28"/>
+      <c r="E161" s="28"/>
+      <c r="F161" s="28"/>
+      <c r="G161" s="28"/>
+      <c r="H161" s="28"/>
+      <c r="I161" s="28"/>
+      <c r="J161" s="6"/>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A162" s="5"/>
+      <c r="B162" s="28"/>
+      <c r="C162" s="28"/>
+      <c r="D162" s="28"/>
+      <c r="E162" s="28"/>
+      <c r="F162" s="28"/>
+      <c r="G162" s="28"/>
+      <c r="H162" s="28"/>
+      <c r="I162" s="28"/>
+      <c r="J162" s="6"/>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A163" s="5"/>
+      <c r="B163" s="28"/>
+      <c r="C163" s="28"/>
+      <c r="D163" s="28"/>
+      <c r="E163" s="28"/>
+      <c r="F163" s="28"/>
+      <c r="G163" s="28"/>
+      <c r="H163" s="28"/>
+      <c r="I163" s="28"/>
+      <c r="J163" s="6"/>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A164" s="5"/>
+      <c r="B164" s="28"/>
+      <c r="C164" s="28"/>
+      <c r="D164" s="28"/>
+      <c r="E164" s="28"/>
+      <c r="F164" s="28"/>
+      <c r="G164" s="28"/>
+      <c r="H164" s="28"/>
+      <c r="I164" s="28"/>
+      <c r="J164" s="6"/>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A165" s="5"/>
+      <c r="B165" s="28"/>
+      <c r="C165" s="28"/>
+      <c r="D165" s="28"/>
+      <c r="E165" s="28"/>
+      <c r="F165" s="28"/>
+      <c r="G165" s="28"/>
+      <c r="H165" s="28"/>
+      <c r="I165" s="28"/>
+      <c r="J165" s="6"/>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A166" s="5"/>
+      <c r="B166" s="28"/>
+      <c r="C166" s="28"/>
+      <c r="D166" s="28"/>
+      <c r="E166" s="28"/>
+      <c r="F166" s="28"/>
+      <c r="G166" s="28"/>
+      <c r="H166" s="28"/>
+      <c r="I166" s="28"/>
+      <c r="J166" s="6"/>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A167" s="5"/>
+      <c r="B167" s="28"/>
+      <c r="C167" s="28"/>
+      <c r="D167" s="28"/>
+      <c r="E167" s="28"/>
+      <c r="F167" s="28"/>
+      <c r="G167" s="28"/>
+      <c r="H167" s="28"/>
+      <c r="I167" s="28"/>
+      <c r="J167" s="6"/>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A168" s="5"/>
+      <c r="B168" s="28"/>
+      <c r="C168" s="28"/>
+      <c r="D168" s="28"/>
+      <c r="E168" s="28"/>
+      <c r="F168" s="28"/>
+      <c r="G168" s="28"/>
+      <c r="H168" s="28"/>
+      <c r="I168" s="28"/>
+      <c r="J168" s="6"/>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A169" s="5"/>
+      <c r="B169" s="28"/>
+      <c r="C169" s="28"/>
+      <c r="D169" s="28"/>
+      <c r="E169" s="28"/>
+      <c r="F169" s="28"/>
+      <c r="G169" s="28"/>
+      <c r="H169" s="28"/>
+      <c r="I169" s="28"/>
+      <c r="J169" s="6"/>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A170" s="5"/>
+      <c r="B170" s="28"/>
+      <c r="C170" s="28"/>
+      <c r="D170" s="28"/>
+      <c r="E170" s="28"/>
+      <c r="F170" s="28"/>
+      <c r="G170" s="28"/>
+      <c r="H170" s="28"/>
+      <c r="I170" s="28"/>
+      <c r="J170" s="6"/>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A171" s="5"/>
+      <c r="B171" s="28"/>
+      <c r="C171" s="28"/>
+      <c r="D171" s="28"/>
+      <c r="E171" s="28"/>
+      <c r="F171" s="28"/>
+      <c r="G171" s="28"/>
+      <c r="H171" s="28"/>
+      <c r="I171" s="28"/>
+      <c r="J171" s="6"/>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A172" s="5"/>
+      <c r="B172" s="28"/>
+      <c r="C172" s="28"/>
+      <c r="D172" s="28"/>
+      <c r="E172" s="28"/>
+      <c r="F172" s="28"/>
+      <c r="G172" s="28"/>
+      <c r="H172" s="28"/>
+      <c r="I172" s="28"/>
+      <c r="J172" s="6"/>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A173" s="5"/>
+      <c r="B173" s="28"/>
+      <c r="C173" s="28"/>
+      <c r="D173" s="28"/>
+      <c r="E173" s="28"/>
+      <c r="F173" s="28"/>
+      <c r="G173" s="28"/>
+      <c r="H173" s="28"/>
+      <c r="I173" s="28"/>
+      <c r="J173" s="6"/>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A174" s="5"/>
+      <c r="B174" s="28"/>
+      <c r="C174" s="28"/>
+      <c r="D174" s="28"/>
+      <c r="E174" s="28"/>
+      <c r="F174" s="28"/>
+      <c r="G174" s="28"/>
+      <c r="H174" s="28"/>
+      <c r="I174" s="28"/>
+      <c r="J174" s="6"/>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A175" s="5"/>
+      <c r="B175" s="28"/>
+      <c r="C175" s="28"/>
+      <c r="D175" s="28"/>
+      <c r="E175" s="28"/>
+      <c r="F175" s="28"/>
+      <c r="G175" s="28"/>
+      <c r="H175" s="28"/>
+      <c r="I175" s="28"/>
+      <c r="J175" s="6"/>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A176" s="5"/>
+      <c r="B176" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="C176" s="28"/>
+      <c r="D176" s="28"/>
+      <c r="E176" s="28"/>
+      <c r="F176" s="28"/>
+      <c r="G176" s="28"/>
+      <c r="H176" s="28"/>
+      <c r="I176" s="28"/>
+      <c r="J176" s="6"/>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A177" s="5"/>
+      <c r="B177" s="28"/>
+      <c r="C177" s="28"/>
+      <c r="D177" s="28"/>
+      <c r="E177" s="28"/>
+      <c r="F177" s="28"/>
+      <c r="G177" s="28"/>
+      <c r="H177" s="28"/>
+      <c r="I177" s="28"/>
+      <c r="J177" s="6"/>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A178" s="5"/>
+      <c r="B178" s="28"/>
+      <c r="C178" s="28"/>
+      <c r="D178" s="28"/>
+      <c r="E178" s="28"/>
+      <c r="F178" s="28"/>
+      <c r="G178" s="28"/>
+      <c r="H178" s="28"/>
+      <c r="I178" s="28"/>
+      <c r="J178" s="6"/>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A179" s="5"/>
+      <c r="B179" s="28"/>
+      <c r="C179" s="28"/>
+      <c r="D179" s="28"/>
+      <c r="E179" s="28"/>
+      <c r="F179" s="28"/>
+      <c r="G179" s="28"/>
+      <c r="H179" s="28"/>
+      <c r="I179" s="28"/>
+      <c r="J179" s="6"/>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A180" s="5"/>
+      <c r="B180" s="28"/>
+      <c r="C180" s="28"/>
+      <c r="D180" s="28"/>
+      <c r="E180" s="28"/>
+      <c r="F180" s="28"/>
+      <c r="G180" s="28"/>
+      <c r="H180" s="28"/>
+      <c r="I180" s="28"/>
+      <c r="J180" s="6"/>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A181" s="5"/>
+      <c r="B181" s="28"/>
+      <c r="C181" s="28"/>
+      <c r="D181" s="28"/>
+      <c r="E181" s="28"/>
+      <c r="F181" s="28"/>
+      <c r="G181" s="28"/>
+      <c r="H181" s="28"/>
+      <c r="I181" s="28"/>
+      <c r="J181" s="6"/>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A182" s="5"/>
+      <c r="B182" s="28"/>
+      <c r="C182" s="28"/>
+      <c r="D182" s="28"/>
+      <c r="E182" s="28"/>
+      <c r="F182" s="28"/>
+      <c r="G182" s="28"/>
+      <c r="H182" s="28"/>
+      <c r="I182" s="28"/>
+      <c r="J182" s="6"/>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A183" s="5"/>
+      <c r="B183" s="28"/>
+      <c r="C183" s="28"/>
+      <c r="D183" s="28"/>
+      <c r="E183" s="28"/>
+      <c r="F183" s="28"/>
+      <c r="G183" s="28"/>
+      <c r="H183" s="28"/>
+      <c r="I183" s="28"/>
+      <c r="J183" s="6"/>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A184" s="5"/>
+      <c r="B184" s="28"/>
+      <c r="C184" s="28"/>
+      <c r="D184" s="28"/>
+      <c r="E184" s="28"/>
+      <c r="F184" s="28"/>
+      <c r="G184" s="28"/>
+      <c r="H184" s="28"/>
+      <c r="I184" s="28"/>
+      <c r="J184" s="6"/>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A185" s="5"/>
+      <c r="B185" s="28"/>
+      <c r="C185" s="28"/>
+      <c r="D185" s="28"/>
+      <c r="E185" s="28"/>
+      <c r="F185" s="28"/>
+      <c r="G185" s="28"/>
+      <c r="H185" s="28"/>
+      <c r="I185" s="28"/>
+      <c r="J185" s="6"/>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A186" s="10"/>
+      <c r="B186" s="11"/>
+      <c r="C186" s="11"/>
+      <c r="D186" s="11"/>
+      <c r="E186" s="11"/>
+      <c r="F186" s="11"/>
+      <c r="G186" s="11"/>
+      <c r="H186" s="11"/>
+      <c r="I186" s="11"/>
+      <c r="J186" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>